<commit_message>
vectors on navbar finished
</commit_message>
<xml_diff>
--- a/public/support files/columns scaffolds.xlsx
+++ b/public/support files/columns scaffolds.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="120">
   <si>
     <t xml:space="preserve">        var dataparameter=[['ChWLDP','left','Chl water temp','smoothedLine']</t>
   </si>
@@ -278,16 +278,131 @@
   </si>
   <si>
     <t>);</t>
+  </si>
+  <si>
+    <t>System</t>
+  </si>
+  <si>
+    <t>Chiller</t>
+  </si>
+  <si>
+    <t>POSSIBLE SYSTEMS - EQUIPMENTS</t>
+  </si>
+  <si>
+    <t>Electric boiler</t>
+  </si>
+  <si>
+    <t>Lighting</t>
+  </si>
+  <si>
+    <t>Heating system</t>
+  </si>
+  <si>
+    <t>Ventilator system</t>
+  </si>
+  <si>
+    <t>Air conditioning system</t>
+  </si>
+  <si>
+    <t>Heating air handle unit</t>
+  </si>
+  <si>
+    <t>Cooling air handle unit</t>
+  </si>
+  <si>
+    <t>Air handle unit variables</t>
+  </si>
+  <si>
+    <t>Outdoor air temperature</t>
+  </si>
+  <si>
+    <t>Mixed air temperature</t>
+  </si>
+  <si>
+    <t>Return air temperature</t>
+  </si>
+  <si>
+    <t>Discharge air temperature</t>
+  </si>
+  <si>
+    <t>Discharge air temperature set point</t>
+  </si>
+  <si>
+    <t>MADamper</t>
+  </si>
+  <si>
+    <t>Mixed air damper position</t>
+  </si>
+  <si>
+    <t>FAN</t>
+  </si>
+  <si>
+    <t>Fan status (on/off)</t>
+  </si>
+  <si>
+    <t>Fan Speed</t>
+  </si>
+  <si>
+    <t>RPM</t>
+  </si>
+  <si>
+    <t>HWV%</t>
+  </si>
+  <si>
+    <t>CWV%</t>
+  </si>
+  <si>
+    <t>Occupancy mode</t>
+  </si>
+  <si>
+    <t>Chilled water valve position</t>
+  </si>
+  <si>
+    <t>Hot water valve position</t>
+  </si>
+  <si>
+    <t>Boiler</t>
+  </si>
+  <si>
+    <t>Common zone</t>
+  </si>
+  <si>
+    <t>Common zone identifier</t>
+  </si>
+  <si>
+    <t>Air handle unit</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>High when occupied, zero if empty</t>
+  </si>
+  <si>
+    <t>On - occupied / off - empty</t>
+  </si>
+  <si>
+    <t>Damper closed while heating or unnocuppied</t>
+  </si>
+  <si>
+    <t>Closed when unnocuppied</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -350,7 +465,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -358,6 +473,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -376,15 +492,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:D33" totalsRowShown="0">
-  <autoFilter ref="A1:D33"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:F33" totalsRowShown="0">
+  <autoFilter ref="A1:F33"/>
+  <tableColumns count="6">
     <tableColumn id="1" name="Column name"/>
     <tableColumn id="2" name="Axis"/>
+    <tableColumn id="5" name="System"/>
     <tableColumn id="3" name="Description"/>
     <tableColumn id="4" name="Chart type">
       <calculatedColumnFormula>IF(B2="left","smoothedLine","column")</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="6" name="Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -653,22 +771,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" customWidth="1"/>
     <col min="2" max="2" width="6.85546875" customWidth="1"/>
-    <col min="3" max="3" width="46.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -676,13 +796,19 @@
         <v>42</v>
       </c>
       <c r="C1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D1" t="s">
         <v>43</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -690,21 +816,24 @@
         <v>40</v>
       </c>
       <c r="C2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" t="s">
         <v>44</v>
       </c>
-      <c r="D2" t="str">
+      <c r="E2" t="str">
         <f>IF(B2="left","smoothedLine","column")</f>
         <v>smoothedLine</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>20</v>
       </c>
-      <c r="G2" t="b">
-        <f>F2=Tabla1[[#This Row],[Column name]]</f>
+      <c r="I2" t="b">
+        <f>H2=Tabla1[[#This Row],[Column name]]</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -712,21 +841,24 @@
         <v>40</v>
       </c>
       <c r="C3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" t="s">
         <v>45</v>
       </c>
-      <c r="D3" t="str">
-        <f t="shared" ref="D3:D33" si="0">IF(B3="left","smoothedLine","column")</f>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E33" si="0">IF(B3="left","smoothedLine","column")</f>
         <v>smoothedLine</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>21</v>
       </c>
-      <c r="G3" t="b">
-        <f>F3=Tabla1[[#This Row],[Column name]]</f>
+      <c r="I3" t="b">
+        <f>H3=Tabla1[[#This Row],[Column name]]</f>
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -734,21 +866,27 @@
         <v>40</v>
       </c>
       <c r="C4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" t="s">
         <v>46</v>
       </c>
-      <c r="D4" t="str">
+      <c r="E4" t="str">
         <f t="shared" si="0"/>
         <v>smoothedLine</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>15</v>
       </c>
-      <c r="G4" t="b">
-        <f>F4=Tabla1[[#This Row],[Column name]]</f>
+      <c r="I4" t="b">
+        <f>H4=Tabla1[[#This Row],[Column name]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -756,21 +894,27 @@
         <v>40</v>
       </c>
       <c r="C5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" t="s">
         <v>47</v>
       </c>
-      <c r="D5" t="str">
+      <c r="E5" t="str">
         <f t="shared" si="0"/>
         <v>smoothedLine</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>14</v>
       </c>
-      <c r="G5" t="b">
-        <f>F5=Tabla1[[#This Row],[Column name]]</f>
+      <c r="I5" t="b">
+        <f>H5=Tabla1[[#This Row],[Column name]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -778,21 +922,27 @@
         <v>40</v>
       </c>
       <c r="C6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" t="s">
         <v>47</v>
       </c>
-      <c r="D6" t="str">
+      <c r="E6" t="str">
         <f t="shared" si="0"/>
         <v>smoothedLine</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>22</v>
       </c>
-      <c r="G6" t="b">
-        <f>F6=Tabla1[[#This Row],[Column name]]</f>
+      <c r="I6" t="b">
+        <f>H6=Tabla1[[#This Row],[Column name]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -800,21 +950,27 @@
         <v>39</v>
       </c>
       <c r="C7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" t="s">
         <v>48</v>
       </c>
-      <c r="D7" t="str">
+      <c r="E7" t="str">
         <f t="shared" si="0"/>
         <v>column</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>12</v>
       </c>
-      <c r="G7" t="b">
-        <f>F7=Tabla1[[#This Row],[Column name]]</f>
+      <c r="I7" t="b">
+        <f>H7=Tabla1[[#This Row],[Column name]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -822,21 +978,24 @@
         <v>40</v>
       </c>
       <c r="C8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D8" t="s">
         <v>55</v>
       </c>
-      <c r="D8" t="str">
+      <c r="E8" t="str">
         <f t="shared" si="0"/>
         <v>smoothedLine</v>
       </c>
-      <c r="F8" t="s">
+      <c r="H8" t="s">
         <v>23</v>
       </c>
-      <c r="G8" t="b">
-        <f>F8=Tabla1[[#This Row],[Column name]]</f>
+      <c r="I8" t="b">
+        <f>H8=Tabla1[[#This Row],[Column name]]</f>
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -844,21 +1003,24 @@
         <v>40</v>
       </c>
       <c r="C9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D9" t="s">
         <v>56</v>
       </c>
-      <c r="D9" t="str">
+      <c r="E9" t="str">
         <f t="shared" si="0"/>
         <v>smoothedLine</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H9" t="s">
         <v>13</v>
       </c>
-      <c r="G9" t="b">
-        <f>F9=Tabla1[[#This Row],[Column name]]</f>
+      <c r="I9" t="b">
+        <f>H9=Tabla1[[#This Row],[Column name]]</f>
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -866,65 +1028,86 @@
         <v>40</v>
       </c>
       <c r="C10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D10" t="s">
         <v>57</v>
       </c>
-      <c r="D10" t="str">
+      <c r="E10" t="str">
         <f t="shared" si="0"/>
         <v>smoothedLine</v>
       </c>
-      <c r="F10" t="s">
+      <c r="H10" t="s">
         <v>24</v>
       </c>
-      <c r="G10" t="b">
-        <f>F10=Tabla1[[#This Row],[Column name]]</f>
+      <c r="I10" t="b">
+        <f>H10=Tabla1[[#This Row],[Column name]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
       <c r="B11" t="s">
         <v>40</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11" t="s">
         <v>49</v>
       </c>
-      <c r="D11" t="str">
+      <c r="E11" t="str">
         <f t="shared" si="0"/>
         <v>smoothedLine</v>
       </c>
       <c r="F11" t="s">
+        <v>116</v>
+      </c>
+      <c r="H11" t="s">
         <v>6</v>
       </c>
-      <c r="G11" t="b">
-        <f>F11=Tabla1[[#This Row],[Column name]]</f>
+      <c r="I11" t="b">
+        <f>H11=Tabla1[[#This Row],[Column name]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
       <c r="B12" t="s">
         <v>40</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" t="s">
         <v>50</v>
       </c>
-      <c r="D12" t="str">
+      <c r="E12" t="str">
         <f t="shared" si="0"/>
         <v>smoothedLine</v>
       </c>
-      <c r="F12" t="s">
+      <c r="H12" t="s">
         <v>25</v>
       </c>
-      <c r="G12" t="b">
-        <f>F12=Tabla1[[#This Row],[Column name]]</f>
+      <c r="I12" t="b">
+        <f>H12=Tabla1[[#This Row],[Column name]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -932,21 +1115,27 @@
         <v>39</v>
       </c>
       <c r="C13" t="s">
+        <v>111</v>
+      </c>
+      <c r="D13" t="s">
         <v>51</v>
       </c>
-      <c r="D13" t="str">
+      <c r="E13" t="str">
         <f t="shared" si="0"/>
         <v>column</v>
       </c>
-      <c r="F13" t="s">
+      <c r="H13" t="s">
         <v>26</v>
       </c>
-      <c r="G13" t="b">
-        <f>F13=Tabla1[[#This Row],[Column name]]</f>
+      <c r="I13" t="b">
+        <f>H13=Tabla1[[#This Row],[Column name]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -954,21 +1143,27 @@
         <v>40</v>
       </c>
       <c r="C14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D14" t="s">
         <v>52</v>
       </c>
-      <c r="D14" t="str">
+      <c r="E14" t="str">
         <f t="shared" si="0"/>
         <v>smoothedLine</v>
       </c>
-      <c r="F14" t="s">
+      <c r="H14" t="s">
         <v>19</v>
       </c>
-      <c r="G14" t="b">
-        <f>F14=Tabla1[[#This Row],[Column name]]</f>
+      <c r="I14" t="b">
+        <f>H14=Tabla1[[#This Row],[Column name]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -976,21 +1171,24 @@
         <v>40</v>
       </c>
       <c r="C15" t="s">
+        <v>111</v>
+      </c>
+      <c r="D15" t="s">
         <v>53</v>
       </c>
-      <c r="D15" t="str">
+      <c r="E15" t="str">
         <f t="shared" si="0"/>
         <v>smoothedLine</v>
       </c>
-      <c r="F15" t="s">
+      <c r="H15" t="s">
         <v>27</v>
       </c>
-      <c r="G15" t="b">
-        <f>F15=Tabla1[[#This Row],[Column name]]</f>
+      <c r="I15" t="b">
+        <f>H15=Tabla1[[#This Row],[Column name]]</f>
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -998,21 +1196,27 @@
         <v>40</v>
       </c>
       <c r="C16" t="s">
+        <v>111</v>
+      </c>
+      <c r="D16" t="s">
         <v>54</v>
       </c>
-      <c r="D16" t="str">
+      <c r="E16" t="str">
         <f t="shared" si="0"/>
         <v>smoothedLine</v>
       </c>
-      <c r="F16" t="s">
+      <c r="H16" t="s">
         <v>18</v>
       </c>
-      <c r="G16" t="b">
-        <f>F16=Tabla1[[#This Row],[Column name]]</f>
+      <c r="I16" t="b">
+        <f>H16=Tabla1[[#This Row],[Column name]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1020,21 +1224,30 @@
         <v>40</v>
       </c>
       <c r="C17" t="s">
+        <v>111</v>
+      </c>
+      <c r="D17" t="s">
         <v>58</v>
       </c>
-      <c r="D17" t="str">
+      <c r="E17" t="str">
         <f t="shared" si="0"/>
         <v>smoothedLine</v>
       </c>
-      <c r="F17" t="s">
+      <c r="H17" t="s">
         <v>17</v>
       </c>
-      <c r="G17" t="b">
-        <f>F17=Tabla1[[#This Row],[Column name]]</f>
+      <c r="I17" t="b">
+        <f>H17=Tabla1[[#This Row],[Column name]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K17" t="s">
+        <v>11</v>
+      </c>
+      <c r="L17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -1042,43 +1255,61 @@
         <v>40</v>
       </c>
       <c r="C18" t="s">
+        <v>111</v>
+      </c>
+      <c r="D18" t="s">
         <v>59</v>
       </c>
-      <c r="D18" t="str">
+      <c r="E18" t="str">
         <f t="shared" si="0"/>
         <v>smoothedLine</v>
       </c>
-      <c r="F18" t="s">
+      <c r="H18" t="s">
         <v>28</v>
       </c>
-      <c r="G18" t="b">
-        <f>F18=Tabla1[[#This Row],[Column name]]</f>
+      <c r="I18" t="b">
+        <f>H18=Tabla1[[#This Row],[Column name]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K18" t="s">
+        <v>10</v>
+      </c>
+      <c r="L18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>10</v>
       </c>
       <c r="B19" t="s">
         <v>40</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D19" t="s">
         <v>60</v>
       </c>
-      <c r="D19" t="str">
+      <c r="E19" t="str">
         <f t="shared" si="0"/>
         <v>smoothedLine</v>
       </c>
-      <c r="F19" t="s">
+      <c r="H19" t="s">
         <v>10</v>
       </c>
-      <c r="G19" t="b">
-        <f>F19=Tabla1[[#This Row],[Column name]]</f>
+      <c r="I19" t="b">
+        <f>H19=Tabla1[[#This Row],[Column name]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K19" t="s">
+        <v>32</v>
+      </c>
+      <c r="L19" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>29</v>
       </c>
@@ -1086,21 +1317,30 @@
         <v>39</v>
       </c>
       <c r="C20" t="s">
+        <v>112</v>
+      </c>
+      <c r="D20" t="s">
         <v>61</v>
       </c>
-      <c r="D20" t="str">
+      <c r="E20" t="str">
         <f t="shared" si="0"/>
         <v>column</v>
       </c>
-      <c r="F20" t="s">
+      <c r="H20" t="s">
         <v>29</v>
       </c>
-      <c r="G20" t="b">
-        <f>F20=Tabla1[[#This Row],[Column name]]</f>
+      <c r="I20" t="b">
+        <f>H20=Tabla1[[#This Row],[Column name]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K20" t="s">
+        <v>13</v>
+      </c>
+      <c r="L20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -1108,43 +1348,64 @@
         <v>39</v>
       </c>
       <c r="C21" t="s">
+        <v>114</v>
+      </c>
+      <c r="D21" t="s">
         <v>62</v>
       </c>
-      <c r="D21" t="str">
+      <c r="E21" t="str">
         <f t="shared" si="0"/>
         <v>column</v>
       </c>
       <c r="F21" t="s">
+        <v>119</v>
+      </c>
+      <c r="H21" t="s">
         <v>30</v>
       </c>
-      <c r="G21" t="b">
-        <f>F21=Tabla1[[#This Row],[Column name]]</f>
+      <c r="I21" t="b">
+        <f>H21=Tabla1[[#This Row],[Column name]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K21" t="s">
+        <v>24</v>
+      </c>
+      <c r="L21" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>31</v>
       </c>
       <c r="B22" t="s">
         <v>39</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D22" t="s">
         <v>63</v>
       </c>
-      <c r="D22" t="str">
+      <c r="E22" t="str">
         <f t="shared" si="0"/>
         <v>column</v>
       </c>
-      <c r="F22" t="s">
+      <c r="H22" t="s">
         <v>31</v>
       </c>
-      <c r="G22" t="b">
-        <f>F22=Tabla1[[#This Row],[Column name]]</f>
+      <c r="I22" t="b">
+        <f>H22=Tabla1[[#This Row],[Column name]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K22" t="s">
+        <v>100</v>
+      </c>
+      <c r="L22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -1152,21 +1413,30 @@
         <v>40</v>
       </c>
       <c r="C23" t="s">
+        <v>112</v>
+      </c>
+      <c r="D23" t="s">
         <v>64</v>
       </c>
-      <c r="D23" t="str">
+      <c r="E23" t="str">
         <f t="shared" si="0"/>
         <v>smoothedLine</v>
       </c>
-      <c r="F23" t="s">
+      <c r="H23" t="s">
         <v>11</v>
       </c>
-      <c r="G23" t="b">
-        <f>F23=Tabla1[[#This Row],[Column name]]</f>
+      <c r="I23" t="b">
+        <f>H23=Tabla1[[#This Row],[Column name]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K23" t="s">
+        <v>102</v>
+      </c>
+      <c r="L23" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -1174,87 +1444,126 @@
         <v>40</v>
       </c>
       <c r="C24" t="s">
+        <v>114</v>
+      </c>
+      <c r="D24" t="s">
         <v>65</v>
       </c>
-      <c r="D24" t="str">
+      <c r="E24" t="str">
         <f t="shared" si="0"/>
         <v>smoothedLine</v>
       </c>
-      <c r="F24" t="s">
+      <c r="H24" t="s">
         <v>32</v>
       </c>
-      <c r="G24" t="b">
-        <f>F24=Tabla1[[#This Row],[Column name]]</f>
+      <c r="I24" t="b">
+        <f>H24=Tabla1[[#This Row],[Column name]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K24" t="s">
+        <v>104</v>
+      </c>
+      <c r="L24" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>33</v>
       </c>
       <c r="B25" t="s">
         <v>40</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D25" t="s">
         <v>66</v>
       </c>
-      <c r="D25" t="str">
+      <c r="E25" t="str">
         <f t="shared" si="0"/>
         <v>smoothedLine</v>
       </c>
       <c r="F25" t="s">
+        <v>116</v>
+      </c>
+      <c r="H25" t="s">
         <v>33</v>
       </c>
-      <c r="G25" t="b">
-        <f>F25=Tabla1[[#This Row],[Column name]]</f>
+      <c r="I25" t="b">
+        <f>H25=Tabla1[[#This Row],[Column name]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K25" t="s">
+        <v>107</v>
+      </c>
+      <c r="L25" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>8</v>
       </c>
       <c r="B26" t="s">
         <v>39</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="D26" t="s">
         <v>67</v>
       </c>
-      <c r="D26" t="str">
+      <c r="E26" t="str">
         <f t="shared" si="0"/>
         <v>column</v>
       </c>
       <c r="F26" t="s">
+        <v>117</v>
+      </c>
+      <c r="H26" t="s">
         <v>8</v>
       </c>
-      <c r="G26" t="b">
-        <f>F26=Tabla1[[#This Row],[Column name]]</f>
+      <c r="I26" t="b">
+        <f>H26=Tabla1[[#This Row],[Column name]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K26" t="s">
+        <v>106</v>
+      </c>
+      <c r="L26" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>34</v>
       </c>
       <c r="B27" t="s">
         <v>39</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>68</v>
       </c>
-      <c r="D27" t="str">
+      <c r="E27" t="str">
         <f t="shared" si="0"/>
         <v>column</v>
       </c>
-      <c r="F27" t="s">
+      <c r="H27" t="s">
         <v>34</v>
       </c>
-      <c r="G27" t="b">
-        <f>F27=Tabla1[[#This Row],[Column name]]</f>
+      <c r="I27" t="b">
+        <f>H27=Tabla1[[#This Row],[Column name]]</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K27" t="s">
+        <v>29</v>
+      </c>
+      <c r="L27" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>35</v>
       </c>
@@ -1262,21 +1571,27 @@
         <v>40</v>
       </c>
       <c r="C28" t="s">
+        <v>114</v>
+      </c>
+      <c r="D28" t="s">
         <v>69</v>
       </c>
-      <c r="D28" t="str">
+      <c r="E28" t="str">
         <f t="shared" si="0"/>
         <v>smoothedLine</v>
       </c>
       <c r="F28" t="s">
+        <v>118</v>
+      </c>
+      <c r="H28" t="s">
         <v>35</v>
       </c>
-      <c r="G28" t="b">
-        <f>F28=Tabla1[[#This Row],[Column name]]</f>
+      <c r="I28" t="b">
+        <f>H28=Tabla1[[#This Row],[Column name]]</f>
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -1284,21 +1599,24 @@
         <v>39</v>
       </c>
       <c r="C29" t="s">
+        <v>112</v>
+      </c>
+      <c r="D29" t="s">
         <v>70</v>
       </c>
-      <c r="D29" t="str">
+      <c r="E29" t="str">
         <f t="shared" si="0"/>
         <v>column</v>
       </c>
-      <c r="F29" t="s">
+      <c r="H29" t="s">
         <v>36</v>
       </c>
-      <c r="G29" t="b">
-        <f>F29=Tabla1[[#This Row],[Column name]]</f>
+      <c r="I29" t="b">
+        <f>H29=Tabla1[[#This Row],[Column name]]</f>
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -1306,21 +1624,24 @@
         <v>39</v>
       </c>
       <c r="C30" t="s">
+        <v>112</v>
+      </c>
+      <c r="D30" t="s">
         <v>71</v>
       </c>
-      <c r="D30" t="str">
+      <c r="E30" t="str">
         <f t="shared" si="0"/>
         <v>column</v>
       </c>
-      <c r="F30" t="s">
+      <c r="H30" t="s">
         <v>7</v>
       </c>
-      <c r="G30" t="b">
-        <f>F30=Tabla1[[#This Row],[Column name]]</f>
+      <c r="I30" t="b">
+        <f>H30=Tabla1[[#This Row],[Column name]]</f>
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -1328,21 +1649,24 @@
         <v>40</v>
       </c>
       <c r="C31" t="s">
+        <v>112</v>
+      </c>
+      <c r="D31" t="s">
         <v>72</v>
       </c>
-      <c r="D31" t="str">
+      <c r="E31" t="str">
         <f t="shared" si="0"/>
         <v>smoothedLine</v>
       </c>
-      <c r="F31" t="s">
+      <c r="H31" t="s">
         <v>9</v>
       </c>
-      <c r="G31" t="b">
-        <f>F31=Tabla1[[#This Row],[Column name]]</f>
+      <c r="I31" t="b">
+        <f>H31=Tabla1[[#This Row],[Column name]]</f>
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -1350,21 +1674,24 @@
         <v>40</v>
       </c>
       <c r="C32" t="s">
+        <v>113</v>
+      </c>
+      <c r="D32" t="s">
         <v>73</v>
       </c>
-      <c r="D32" t="str">
+      <c r="E32" t="str">
         <f t="shared" si="0"/>
         <v>smoothedLine</v>
       </c>
-      <c r="F32" t="s">
+      <c r="H32" t="s">
         <v>37</v>
       </c>
-      <c r="G32" t="b">
-        <f>F32=Tabla1[[#This Row],[Column name]]</f>
+      <c r="I32" t="b">
+        <f>H32=Tabla1[[#This Row],[Column name]]</f>
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -1372,24 +1699,28 @@
         <v>40</v>
       </c>
       <c r="C33" t="s">
+        <v>114</v>
+      </c>
+      <c r="D33" t="s">
         <v>74</v>
       </c>
-      <c r="D33" t="str">
+      <c r="E33" t="str">
         <f t="shared" si="0"/>
         <v>smoothedLine</v>
       </c>
-      <c r="F33" t="s">
+      <c r="H33" t="s">
         <v>38</v>
       </c>
-      <c r="G33" t="b">
-        <f>F33=Tabla1[[#This Row],[Column name]]</f>
+      <c r="I33" t="b">
+        <f>H33=Tabla1[[#This Row],[Column name]]</f>
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1428,7 +1759,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
-        <f>$A$1&amp;'codes and names'!C2&amp;$B$1</f>
+        <f>$A$1&amp;'codes and names'!D2&amp;$B$1</f>
         <v>&lt;th&gt;Chilled-Water Loop Differential Pressure&lt;/th&gt;</v>
       </c>
       <c r="B4" t="str">
@@ -1450,7 +1781,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="str">
-        <f>$A$1&amp;'codes and names'!C3&amp;$B$1</f>
+        <f>$A$1&amp;'codes and names'!D3&amp;$B$1</f>
         <v>&lt;th&gt;Chilled-Water Loop Differential Pressure Set Point&lt;/th&gt;</v>
       </c>
       <c r="B5" s="5" t="str">
@@ -1472,7 +1803,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="str">
-        <f>$A$1&amp;'codes and names'!C4&amp;$B$1</f>
+        <f>$A$1&amp;'codes and names'!D4&amp;$B$1</f>
         <v>&lt;th&gt;Chilled-Water Return Temp&lt;/th&gt;</v>
       </c>
       <c r="B6" s="5" t="str">
@@ -1494,7 +1825,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="str">
-        <f>$A$1&amp;'codes and names'!C5&amp;$B$1</f>
+        <f>$A$1&amp;'codes and names'!D5&amp;$B$1</f>
         <v>&lt;th&gt;Chilled-Water Supply Temp&lt;/th&gt;</v>
       </c>
       <c r="B7" s="5" t="str">
@@ -1516,7 +1847,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="str">
-        <f>$A$1&amp;'codes and names'!C6&amp;$B$1</f>
+        <f>$A$1&amp;'codes and names'!D6&amp;$B$1</f>
         <v>&lt;th&gt;Chilled-Water Supply Temp&lt;/th&gt;</v>
       </c>
       <c r="B8" s="5" t="str">
@@ -1538,7 +1869,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="str">
-        <f>$A$1&amp;'codes and names'!C7&amp;$B$1</f>
+        <f>$A$1&amp;'codes and names'!D7&amp;$B$1</f>
         <v>&lt;th&gt;Cooling-Coil Valve Signal (%)&lt;/th&gt;</v>
       </c>
       <c r="B9" s="5" t="str">
@@ -1560,7 +1891,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="str">
-        <f>$A$1&amp;'codes and names'!C8&amp;$B$1</f>
+        <f>$A$1&amp;'codes and names'!D8&amp;$B$1</f>
         <v>&lt;th&gt;Consumption kWH&lt;/th&gt;</v>
       </c>
       <c r="B10" s="5" t="str">
@@ -1582,7 +1913,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="str">
-        <f>$A$1&amp;'codes and names'!C9&amp;$B$1</f>
+        <f>$A$1&amp;'codes and names'!D9&amp;$B$1</f>
         <v>&lt;th&gt;Discharge-Air Temp&lt;/th&gt;</v>
       </c>
       <c r="B11" s="5" t="str">
@@ -1604,7 +1935,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="str">
-        <f>$A$1&amp;'codes and names'!C10&amp;$B$1</f>
+        <f>$A$1&amp;'codes and names'!D10&amp;$B$1</f>
         <v>&lt;th&gt;Discharge-Air Temp Set Point&lt;/th&gt;</v>
       </c>
       <c r="B12" s="5" t="str">
@@ -1626,7 +1957,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="str">
-        <f>$A$1&amp;'codes and names'!C11&amp;$B$1</f>
+        <f>$A$1&amp;'codes and names'!D11&amp;$B$1</f>
         <v>&lt;th&gt;Duct Static Pressure&lt;/th&gt;</v>
       </c>
       <c r="B13" s="5" t="str">
@@ -1648,7 +1979,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="str">
-        <f>$A$1&amp;'codes and names'!C12&amp;$B$1</f>
+        <f>$A$1&amp;'codes and names'!D12&amp;$B$1</f>
         <v>&lt;th&gt;Duct Static Pressure Set Point&lt;/th&gt;</v>
       </c>
       <c r="B14" s="5" t="str">
@@ -1670,7 +2001,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="str">
-        <f>$A$1&amp;'codes and names'!C13&amp;$B$1</f>
+        <f>$A$1&amp;'codes and names'!D13&amp;$B$1</f>
         <v>&lt;th&gt;Heating-Coil Valve Signal (%)&lt;/th&gt;</v>
       </c>
       <c r="B15" s="5" t="str">
@@ -1692,7 +2023,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="str">
-        <f>$A$1&amp;'codes and names'!C14&amp;$B$1</f>
+        <f>$A$1&amp;'codes and names'!D14&amp;$B$1</f>
         <v>&lt;th&gt;Hot-Water Loop Differential Pressure&lt;/th&gt;</v>
       </c>
       <c r="B16" s="5" t="str">
@@ -1714,7 +2045,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="str">
-        <f>$A$1&amp;'codes and names'!C15&amp;$B$1</f>
+        <f>$A$1&amp;'codes and names'!D15&amp;$B$1</f>
         <v>&lt;th&gt;Hot-Water Loop Differential Pressure Set Point&lt;/th&gt;</v>
       </c>
       <c r="B17" s="5" t="str">
@@ -1736,7 +2067,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="str">
-        <f>$A$1&amp;'codes and names'!C16&amp;$B$1</f>
+        <f>$A$1&amp;'codes and names'!D16&amp;$B$1</f>
         <v>&lt;th&gt;Hot-Water Return Temp&lt;/th&gt;</v>
       </c>
       <c r="B18" s="5" t="str">
@@ -1758,7 +2089,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="str">
-        <f>$A$1&amp;'codes and names'!C17&amp;$B$1</f>
+        <f>$A$1&amp;'codes and names'!D17&amp;$B$1</f>
         <v>&lt;th&gt;Hot-Water Supply Temp&lt;/th&gt;</v>
       </c>
       <c r="B19" s="5" t="str">
@@ -1780,7 +2111,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="str">
-        <f>$A$1&amp;'codes and names'!C18&amp;$B$1</f>
+        <f>$A$1&amp;'codes and names'!D18&amp;$B$1</f>
         <v>&lt;th&gt;Hot-Water Supply Temp Set Point&lt;/th&gt;</v>
       </c>
       <c r="B20" s="5" t="str">
@@ -1802,7 +2133,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="str">
-        <f>$A$1&amp;'codes and names'!C19&amp;$B$1</f>
+        <f>$A$1&amp;'codes and names'!D19&amp;$B$1</f>
         <v>&lt;th&gt;Mixed-Air Temp&lt;/th&gt;</v>
       </c>
       <c r="B21" s="5" t="str">
@@ -1824,7 +2155,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="str">
-        <f>$A$1&amp;'codes and names'!C20&amp;$B$1</f>
+        <f>$A$1&amp;'codes and names'!D20&amp;$B$1</f>
         <v>&lt;th&gt;Occupancy Mode&lt;/th&gt;</v>
       </c>
       <c r="B22" s="5" t="str">
@@ -1846,7 +2177,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="str">
-        <f>$A$1&amp;'codes and names'!C21&amp;$B$1</f>
+        <f>$A$1&amp;'codes and names'!D21&amp;$B$1</f>
         <v>&lt;th&gt;Outdoor-Air Damper Position Signal (%)&lt;/th&gt;</v>
       </c>
       <c r="B23" s="5" t="str">
@@ -1868,7 +2199,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="str">
-        <f>$A$1&amp;'codes and names'!C22&amp;$B$1</f>
+        <f>$A$1&amp;'codes and names'!D22&amp;$B$1</f>
         <v>&lt;th&gt;Outdoor-Air Fraction temp&lt;/th&gt;</v>
       </c>
       <c r="B24" s="5" t="str">
@@ -1890,7 +2221,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="str">
-        <f>$A$1&amp;'codes and names'!C23&amp;$B$1</f>
+        <f>$A$1&amp;'codes and names'!D23&amp;$B$1</f>
         <v>&lt;th&gt;Outdoor-Air Temp (temp)&lt;/th&gt;</v>
       </c>
       <c r="B25" s="5" t="str">
@@ -1912,7 +2243,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="str">
-        <f>$A$1&amp;'codes and names'!C24&amp;$B$1</f>
+        <f>$A$1&amp;'codes and names'!D24&amp;$B$1</f>
         <v>&lt;th&gt;Return-Air Temp&lt;/th&gt;</v>
       </c>
       <c r="B26" s="6" t="str">
@@ -1934,7 +2265,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="str">
-        <f>$A$1&amp;'codes and names'!C25&amp;$B$1</f>
+        <f>$A$1&amp;'codes and names'!D25&amp;$B$1</f>
         <v>&lt;th&gt;Supply-Fan Speed&lt;/th&gt;</v>
       </c>
       <c r="B27" s="6" t="str">
@@ -1956,7 +2287,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="str">
-        <f>$A$1&amp;'codes and names'!C26&amp;$B$1</f>
+        <f>$A$1&amp;'codes and names'!D26&amp;$B$1</f>
         <v>&lt;th&gt;Supply Fan Status (on/off)&lt;/th&gt;</v>
       </c>
       <c r="B28" s="6" t="str">
@@ -1978,7 +2309,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="str">
-        <f>$A$1&amp;'codes and names'!C27&amp;$B$1</f>
+        <f>$A$1&amp;'codes and names'!D27&amp;$B$1</f>
         <v>&lt;th&gt;VAV Damper Position Set Point (%)&lt;/th&gt;</v>
       </c>
       <c r="B29" s="6" t="str">
@@ -2000,7 +2331,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="str">
-        <f>$A$1&amp;'codes and names'!C28&amp;$B$1</f>
+        <f>$A$1&amp;'codes and names'!D28&amp;$B$1</f>
         <v>&lt;th&gt;Zone Damper Position Signal (%)&lt;/th&gt;</v>
       </c>
       <c r="B30" s="6" t="str">
@@ -2022,7 +2353,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="str">
-        <f>$A$1&amp;'codes and names'!C29&amp;$B$1</f>
+        <f>$A$1&amp;'codes and names'!D29&amp;$B$1</f>
         <v>&lt;th&gt;Zone Occupancy Mode (Occupied/Unoccupied)&lt;/th&gt;</v>
       </c>
       <c r="B31" s="6" t="str">
@@ -2044,7 +2375,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="str">
-        <f>$A$1&amp;'codes and names'!C30&amp;$B$1</f>
+        <f>$A$1&amp;'codes and names'!D30&amp;$B$1</f>
         <v>&lt;th&gt;Zone Reheat Valve Signal (%)&lt;/th&gt;</v>
       </c>
       <c r="B32" s="6" t="str">
@@ -2066,7 +2397,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="str">
-        <f>$A$1&amp;'codes and names'!C31&amp;$B$1</f>
+        <f>$A$1&amp;'codes and names'!D31&amp;$B$1</f>
         <v>&lt;th&gt;Zone Temperature&lt;/th&gt;</v>
       </c>
       <c r="B33" s="6" t="str">
@@ -2088,7 +2419,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="str">
-        <f>$A$1&amp;'codes and names'!C32&amp;$B$1</f>
+        <f>$A$1&amp;'codes and names'!D32&amp;$B$1</f>
         <v>&lt;th&gt;Zone&lt;/th&gt;</v>
       </c>
       <c r="B34" s="6" t="str">
@@ -2110,7 +2441,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="str">
-        <f>$A$1&amp;'codes and names'!C33&amp;$B$1</f>
+        <f>$A$1&amp;'codes and names'!D33&amp;$B$1</f>
         <v>&lt;th&gt;Damper&lt;/th&gt;</v>
       </c>
       <c r="B35" s="6" t="str">
@@ -2207,7 +2538,7 @@
       </c>
       <c r="B11" t="str">
         <f>$A$1&amp;A11&amp;$A$2&amp;AB11&amp;AC11&amp;AD11&amp;AE11&amp;AF11&amp;$A$3</f>
-        <v>if ($('#dparameters').html().trim()==1) { var dataparameter=[['ZT','left','Zone Temperature','smoothedLine'],['ZRVS','right','Zone Reheat Valve Signal (%)','column'],['ZOM','right','Zone Occupancy Mode (Occupied/Unoccupied)','column']]; }</v>
+        <v>if ($('#dparameters').html().trim()==1) { var dataparameter=[['ZT','left','Common zone','Zone Temperature'],['ZRVS','right','Common zone','Zone Reheat Valve Signal (%)'],['ZOM','right','Common zone','Zone Occupancy Mode (Occupied/Unoccupied)']]; }</v>
       </c>
       <c r="H11" t="s">
         <v>9</v>
@@ -2240,15 +2571,15 @@
       </c>
       <c r="R11" s="4" t="str">
         <f>IF(H11&lt;&gt;"",VLOOKUP(H11,Tabla1[#All],3,FALSE),"")</f>
-        <v>Zone Temperature</v>
+        <v>Common zone</v>
       </c>
       <c r="S11" s="4" t="str">
         <f>IF(I11&lt;&gt;"",VLOOKUP(I11,Tabla1[#All],3,FALSE),"")</f>
-        <v>Zone Reheat Valve Signal (%)</v>
+        <v>Common zone</v>
       </c>
       <c r="T11" s="4" t="str">
         <f>IF(J11&lt;&gt;"",VLOOKUP(J11,Tabla1[#All],3,FALSE),"")</f>
-        <v>Zone Occupancy Mode (Occupied/Unoccupied)</v>
+        <v>Common zone</v>
       </c>
       <c r="U11" s="4" t="str">
         <f>IF(K11&lt;&gt;"",VLOOKUP(K11,Tabla1[#All],3,FALSE),"")</f>
@@ -2260,15 +2591,15 @@
       </c>
       <c r="W11" s="1" t="str">
         <f>IF(H11&lt;&gt;"",VLOOKUP(H11,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Zone Temperature</v>
       </c>
       <c r="X11" s="1" t="str">
         <f>IF(I11&lt;&gt;"",VLOOKUP(I11,Tabla1[#All],4,FALSE),"")</f>
-        <v>column</v>
+        <v>Zone Reheat Valve Signal (%)</v>
       </c>
       <c r="Y11" s="1" t="str">
         <f>IF(J11&lt;&gt;"",VLOOKUP(J11,Tabla1[#All],4,FALSE),"")</f>
-        <v>column</v>
+        <v>Zone Occupancy Mode (Occupied/Unoccupied)</v>
       </c>
       <c r="Z11" s="1" t="str">
         <f>IF(K11&lt;&gt;"",VLOOKUP(K11,Tabla1[#All],4,FALSE),"")</f>
@@ -2280,15 +2611,15 @@
       </c>
       <c r="AB11" s="3" t="str">
         <f>"['"&amp;H11&amp;"','"&amp;M11&amp;"','"&amp;R11&amp;"','"&amp;W11&amp;"']"</f>
-        <v>['ZT','left','Zone Temperature','smoothedLine']</v>
+        <v>['ZT','left','Common zone','Zone Temperature']</v>
       </c>
       <c r="AC11" s="3" t="str">
         <f>IF(I11&lt;&gt;"",",['"&amp;I11&amp;"','"&amp;N11&amp;"','"&amp;S11&amp;"','"&amp;X11&amp;"']","")</f>
-        <v>,['ZRVS','right','Zone Reheat Valve Signal (%)','column']</v>
+        <v>,['ZRVS','right','Common zone','Zone Reheat Valve Signal (%)']</v>
       </c>
       <c r="AD11" s="3" t="str">
         <f>IF(J11&lt;&gt;"",",['"&amp;J11&amp;"','"&amp;O11&amp;"','"&amp;T11&amp;"','"&amp;Y11&amp;"']","")</f>
-        <v>,['ZOM','right','Zone Occupancy Mode (Occupied/Unoccupied)','column']</v>
+        <v>,['ZOM','right','Common zone','Zone Occupancy Mode (Occupied/Unoccupied)']</v>
       </c>
       <c r="AE11" s="3" t="str">
         <f>IF(K11&lt;&gt;"",",['"&amp;K11&amp;"','"&amp;P11&amp;"','"&amp;U11&amp;"','"&amp;Z11&amp;"']","")</f>
@@ -2305,7 +2636,7 @@
       </c>
       <c r="B12" t="str">
         <f t="shared" ref="B12:B38" si="0">$A$1&amp;A12&amp;$A$2&amp;AB12&amp;AC12&amp;AD12&amp;AE12&amp;AF12&amp;$A$3</f>
-        <v>if ($('#dparameters').html().trim()==2) { var dataparameter=[['ZT','left','Zone Temperature','smoothedLine'],['ZRVS','right','Zone Reheat Valve Signal (%)','column'],['OAT','left','Outdoor-Air Temp (temp)','smoothedLine']]; }</v>
+        <v>if ($('#dparameters').html().trim()==2) { var dataparameter=[['ZT','left','Common zone','Zone Temperature'],['ZRVS','right','Common zone','Zone Reheat Valve Signal (%)'],['OAT','left','Common zone','Outdoor-Air Temp (temp)']]; }</v>
       </c>
       <c r="H12" t="s">
         <v>9</v>
@@ -2338,15 +2669,15 @@
       </c>
       <c r="R12" s="4" t="str">
         <f>IF(H12&lt;&gt;"",VLOOKUP(H12,Tabla1[#All],3,FALSE),"")</f>
-        <v>Zone Temperature</v>
+        <v>Common zone</v>
       </c>
       <c r="S12" s="4" t="str">
         <f>IF(I12&lt;&gt;"",VLOOKUP(I12,Tabla1[#All],3,FALSE),"")</f>
-        <v>Zone Reheat Valve Signal (%)</v>
+        <v>Common zone</v>
       </c>
       <c r="T12" s="4" t="str">
         <f>IF(J12&lt;&gt;"",VLOOKUP(J12,Tabla1[#All],3,FALSE),"")</f>
-        <v>Outdoor-Air Temp (temp)</v>
+        <v>Common zone</v>
       </c>
       <c r="U12" s="4" t="str">
         <f>IF(K12&lt;&gt;"",VLOOKUP(K12,Tabla1[#All],3,FALSE),"")</f>
@@ -2358,15 +2689,15 @@
       </c>
       <c r="W12" s="1" t="str">
         <f>IF(H12&lt;&gt;"",VLOOKUP(H12,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Zone Temperature</v>
       </c>
       <c r="X12" s="1" t="str">
         <f>IF(I12&lt;&gt;"",VLOOKUP(I12,Tabla1[#All],4,FALSE),"")</f>
-        <v>column</v>
+        <v>Zone Reheat Valve Signal (%)</v>
       </c>
       <c r="Y12" s="1" t="str">
         <f>IF(J12&lt;&gt;"",VLOOKUP(J12,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Outdoor-Air Temp (temp)</v>
       </c>
       <c r="Z12" s="1" t="str">
         <f>IF(K12&lt;&gt;"",VLOOKUP(K12,Tabla1[#All],4,FALSE),"")</f>
@@ -2378,15 +2709,15 @@
       </c>
       <c r="AB12" s="3" t="str">
         <f t="shared" ref="AB12:AB38" si="1">"['"&amp;H12&amp;"','"&amp;M12&amp;"','"&amp;R12&amp;"','"&amp;W12&amp;"']"</f>
-        <v>['ZT','left','Zone Temperature','smoothedLine']</v>
+        <v>['ZT','left','Common zone','Zone Temperature']</v>
       </c>
       <c r="AC12" s="3" t="str">
         <f t="shared" ref="AC12:AF38" si="2">IF(I12&lt;&gt;"",",['"&amp;I12&amp;"','"&amp;N12&amp;"','"&amp;S12&amp;"','"&amp;X12&amp;"']","")</f>
-        <v>,['ZRVS','right','Zone Reheat Valve Signal (%)','column']</v>
+        <v>,['ZRVS','right','Common zone','Zone Reheat Valve Signal (%)']</v>
       </c>
       <c r="AD12" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>,['OAT','left','Outdoor-Air Temp (temp)','smoothedLine']</v>
+        <v>,['OAT','left','Common zone','Outdoor-Air Temp (temp)']</v>
       </c>
       <c r="AE12" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2403,7 +2734,7 @@
       </c>
       <c r="B13" t="str">
         <f t="shared" si="0"/>
-        <v>if ($('#dparameters').html().trim()==3) { var dataparameter=[['MAT','left','Mixed-Air Temp','smoothedLine'],['OADPS','right','Outdoor-Air Damper Position Signal (%)','column'],['OAF','right','Outdoor-Air Fraction temp','column'],['OAT','left','Outdoor-Air Temp (temp)','smoothedLine'],['RAT','left','Return-Air Temp','smoothedLine']]; }</v>
+        <v>if ($('#dparameters').html().trim()==3) { var dataparameter=[['MAT','left','Air handle unit','Mixed-Air Temp'],['OADPS','right','Air handle unit','Outdoor-Air Damper Position Signal (%)'],['OAF','right','Air handle unit','Outdoor-Air Fraction temp'],['OAT','left','Common zone','Outdoor-Air Temp (temp)'],['RAT','left','Air handle unit','Return-Air Temp']]; }</v>
       </c>
       <c r="H13" t="s">
         <v>10</v>
@@ -2442,63 +2773,63 @@
       </c>
       <c r="R13" s="4" t="str">
         <f>IF(H13&lt;&gt;"",VLOOKUP(H13,Tabla1[#All],3,FALSE),"")</f>
-        <v>Mixed-Air Temp</v>
+        <v>Air handle unit</v>
       </c>
       <c r="S13" s="4" t="str">
         <f>IF(I13&lt;&gt;"",VLOOKUP(I13,Tabla1[#All],3,FALSE),"")</f>
-        <v>Outdoor-Air Damper Position Signal (%)</v>
+        <v>Air handle unit</v>
       </c>
       <c r="T13" s="4" t="str">
         <f>IF(J13&lt;&gt;"",VLOOKUP(J13,Tabla1[#All],3,FALSE),"")</f>
-        <v>Outdoor-Air Fraction temp</v>
+        <v>Air handle unit</v>
       </c>
       <c r="U13" s="4" t="str">
         <f>IF(K13&lt;&gt;"",VLOOKUP(K13,Tabla1[#All],3,FALSE),"")</f>
-        <v>Outdoor-Air Temp (temp)</v>
+        <v>Common zone</v>
       </c>
       <c r="V13" s="4" t="str">
         <f>IF(L13&lt;&gt;"",VLOOKUP(L13,Tabla1[#All],3,FALSE),"")</f>
-        <v>Return-Air Temp</v>
+        <v>Air handle unit</v>
       </c>
       <c r="W13" s="1" t="str">
         <f>IF(H13&lt;&gt;"",VLOOKUP(H13,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Mixed-Air Temp</v>
       </c>
       <c r="X13" s="1" t="str">
         <f>IF(I13&lt;&gt;"",VLOOKUP(I13,Tabla1[#All],4,FALSE),"")</f>
-        <v>column</v>
+        <v>Outdoor-Air Damper Position Signal (%)</v>
       </c>
       <c r="Y13" s="1" t="str">
         <f>IF(J13&lt;&gt;"",VLOOKUP(J13,Tabla1[#All],4,FALSE),"")</f>
-        <v>column</v>
+        <v>Outdoor-Air Fraction temp</v>
       </c>
       <c r="Z13" s="1" t="str">
         <f>IF(K13&lt;&gt;"",VLOOKUP(K13,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Outdoor-Air Temp (temp)</v>
       </c>
       <c r="AA13" s="1" t="str">
         <f>IF(L13&lt;&gt;"",VLOOKUP(L13,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Return-Air Temp</v>
       </c>
       <c r="AB13" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>['MAT','left','Mixed-Air Temp','smoothedLine']</v>
+        <v>['MAT','left','Air handle unit','Mixed-Air Temp']</v>
       </c>
       <c r="AC13" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>,['OADPS','right','Outdoor-Air Damper Position Signal (%)','column']</v>
+        <v>,['OADPS','right','Air handle unit','Outdoor-Air Damper Position Signal (%)']</v>
       </c>
       <c r="AD13" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>,['OAF','right','Outdoor-Air Fraction temp','column']</v>
+        <v>,['OAF','right','Air handle unit','Outdoor-Air Fraction temp']</v>
       </c>
       <c r="AE13" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>,['OAT','left','Outdoor-Air Temp (temp)','smoothedLine']</v>
+        <v>,['OAT','left','Common zone','Outdoor-Air Temp (temp)']</v>
       </c>
       <c r="AF13" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>,['RAT','left','Return-Air Temp','smoothedLine']</v>
+        <v>,['RAT','left','Air handle unit','Return-Air Temp']</v>
       </c>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
@@ -2507,7 +2838,7 @@
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
-        <v>if ($('#dparameters').html().trim()==4) { var dataparameter=[['OAT','left','Outdoor-Air Temp (temp)','smoothedLine'],['OADPS','right','Outdoor-Air Damper Position Signal (%)','column'],['OAF','right','Outdoor-Air Fraction temp','column']]; }</v>
+        <v>if ($('#dparameters').html().trim()==4) { var dataparameter=[['OAT','left','Common zone','Outdoor-Air Temp (temp)'],['OADPS','right','Air handle unit','Outdoor-Air Damper Position Signal (%)'],['OAF','right','Air handle unit','Outdoor-Air Fraction temp']]; }</v>
       </c>
       <c r="H14" t="s">
         <v>11</v>
@@ -2540,15 +2871,15 @@
       </c>
       <c r="R14" s="4" t="str">
         <f>IF(H14&lt;&gt;"",VLOOKUP(H14,Tabla1[#All],3,FALSE),"")</f>
-        <v>Outdoor-Air Temp (temp)</v>
+        <v>Common zone</v>
       </c>
       <c r="S14" s="4" t="str">
         <f>IF(I14&lt;&gt;"",VLOOKUP(I14,Tabla1[#All],3,FALSE),"")</f>
-        <v>Outdoor-Air Damper Position Signal (%)</v>
+        <v>Air handle unit</v>
       </c>
       <c r="T14" s="4" t="str">
         <f>IF(J14&lt;&gt;"",VLOOKUP(J14,Tabla1[#All],3,FALSE),"")</f>
-        <v>Outdoor-Air Fraction temp</v>
+        <v>Air handle unit</v>
       </c>
       <c r="U14" s="4" t="str">
         <f>IF(K14&lt;&gt;"",VLOOKUP(K14,Tabla1[#All],3,FALSE),"")</f>
@@ -2560,15 +2891,15 @@
       </c>
       <c r="W14" s="1" t="str">
         <f>IF(H14&lt;&gt;"",VLOOKUP(H14,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Outdoor-Air Temp (temp)</v>
       </c>
       <c r="X14" s="1" t="str">
         <f>IF(I14&lt;&gt;"",VLOOKUP(I14,Tabla1[#All],4,FALSE),"")</f>
-        <v>column</v>
+        <v>Outdoor-Air Damper Position Signal (%)</v>
       </c>
       <c r="Y14" s="1" t="str">
         <f>IF(J14&lt;&gt;"",VLOOKUP(J14,Tabla1[#All],4,FALSE),"")</f>
-        <v>column</v>
+        <v>Outdoor-Air Fraction temp</v>
       </c>
       <c r="Z14" s="1" t="str">
         <f>IF(K14&lt;&gt;"",VLOOKUP(K14,Tabla1[#All],4,FALSE),"")</f>
@@ -2580,15 +2911,15 @@
       </c>
       <c r="AB14" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>['OAT','left','Outdoor-Air Temp (temp)','smoothedLine']</v>
+        <v>['OAT','left','Common zone','Outdoor-Air Temp (temp)']</v>
       </c>
       <c r="AC14" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>,['OADPS','right','Outdoor-Air Damper Position Signal (%)','column']</v>
+        <v>,['OADPS','right','Air handle unit','Outdoor-Air Damper Position Signal (%)']</v>
       </c>
       <c r="AD14" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>,['OAF','right','Outdoor-Air Fraction temp','column']</v>
+        <v>,['OAF','right','Air handle unit','Outdoor-Air Fraction temp']</v>
       </c>
       <c r="AE14" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2605,7 +2936,7 @@
       </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>
-        <v>if ($('#dparameters').html().trim()==5) { var dataparameter=[['OAT','left','Outdoor-Air Temp (temp)','smoothedLine'],['RAT','left','Return-Air Temp','smoothedLine'],['OADPS','right','Outdoor-Air Damper Position Signal (%)','column']]; }</v>
+        <v>if ($('#dparameters').html().trim()==5) { var dataparameter=[['OAT','left','Common zone','Outdoor-Air Temp (temp)'],['RAT','left','Air handle unit','Return-Air Temp'],['OADPS','right','Air handle unit','Outdoor-Air Damper Position Signal (%)']]; }</v>
       </c>
       <c r="H15" t="s">
         <v>11</v>
@@ -2638,15 +2969,15 @@
       </c>
       <c r="R15" s="4" t="str">
         <f>IF(H15&lt;&gt;"",VLOOKUP(H15,Tabla1[#All],3,FALSE),"")</f>
-        <v>Outdoor-Air Temp (temp)</v>
+        <v>Common zone</v>
       </c>
       <c r="S15" s="4" t="str">
         <f>IF(I15&lt;&gt;"",VLOOKUP(I15,Tabla1[#All],3,FALSE),"")</f>
-        <v>Return-Air Temp</v>
+        <v>Air handle unit</v>
       </c>
       <c r="T15" s="4" t="str">
         <f>IF(J15&lt;&gt;"",VLOOKUP(J15,Tabla1[#All],3,FALSE),"")</f>
-        <v>Outdoor-Air Damper Position Signal (%)</v>
+        <v>Air handle unit</v>
       </c>
       <c r="U15" s="4" t="str">
         <f>IF(K15&lt;&gt;"",VLOOKUP(K15,Tabla1[#All],3,FALSE),"")</f>
@@ -2658,15 +2989,15 @@
       </c>
       <c r="W15" s="1" t="str">
         <f>IF(H15&lt;&gt;"",VLOOKUP(H15,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Outdoor-Air Temp (temp)</v>
       </c>
       <c r="X15" s="1" t="str">
         <f>IF(I15&lt;&gt;"",VLOOKUP(I15,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Return-Air Temp</v>
       </c>
       <c r="Y15" s="1" t="str">
         <f>IF(J15&lt;&gt;"",VLOOKUP(J15,Tabla1[#All],4,FALSE),"")</f>
-        <v>column</v>
+        <v>Outdoor-Air Damper Position Signal (%)</v>
       </c>
       <c r="Z15" s="1" t="str">
         <f>IF(K15&lt;&gt;"",VLOOKUP(K15,Tabla1[#All],4,FALSE),"")</f>
@@ -2678,15 +3009,15 @@
       </c>
       <c r="AB15" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>['OAT','left','Outdoor-Air Temp (temp)','smoothedLine']</v>
+        <v>['OAT','left','Common zone','Outdoor-Air Temp (temp)']</v>
       </c>
       <c r="AC15" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>,['RAT','left','Return-Air Temp','smoothedLine']</v>
+        <v>,['RAT','left','Air handle unit','Return-Air Temp']</v>
       </c>
       <c r="AD15" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>,['OADPS','right','Outdoor-Air Damper Position Signal (%)','column']</v>
+        <v>,['OADPS','right','Air handle unit','Outdoor-Air Damper Position Signal (%)']</v>
       </c>
       <c r="AE15" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2703,7 +3034,7 @@
       </c>
       <c r="B16" t="str">
         <f t="shared" si="0"/>
-        <v>if ($('#dparameters').html().trim()==6) { var dataparameter=[['OAT','left','Outdoor-Air Temp (temp)','smoothedLine'],['OADPS','right','Outdoor-Air Damper Position Signal (%)','column']]; }</v>
+        <v>if ($('#dparameters').html().trim()==6) { var dataparameter=[['OAT','left','Common zone','Outdoor-Air Temp (temp)'],['OADPS','right','Air handle unit','Outdoor-Air Damper Position Signal (%)']]; }</v>
       </c>
       <c r="H16" t="s">
         <v>11</v>
@@ -2733,11 +3064,11 @@
       </c>
       <c r="R16" s="4" t="str">
         <f>IF(H16&lt;&gt;"",VLOOKUP(H16,Tabla1[#All],3,FALSE),"")</f>
-        <v>Outdoor-Air Temp (temp)</v>
+        <v>Common zone</v>
       </c>
       <c r="S16" s="4" t="str">
         <f>IF(I16&lt;&gt;"",VLOOKUP(I16,Tabla1[#All],3,FALSE),"")</f>
-        <v>Outdoor-Air Damper Position Signal (%)</v>
+        <v>Air handle unit</v>
       </c>
       <c r="T16" s="4" t="str">
         <f>IF(J16&lt;&gt;"",VLOOKUP(J16,Tabla1[#All],3,FALSE),"")</f>
@@ -2753,11 +3084,11 @@
       </c>
       <c r="W16" s="1" t="str">
         <f>IF(H16&lt;&gt;"",VLOOKUP(H16,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Outdoor-Air Temp (temp)</v>
       </c>
       <c r="X16" s="1" t="str">
         <f>IF(I16&lt;&gt;"",VLOOKUP(I16,Tabla1[#All],4,FALSE),"")</f>
-        <v>column</v>
+        <v>Outdoor-Air Damper Position Signal (%)</v>
       </c>
       <c r="Y16" s="1" t="str">
         <f>IF(J16&lt;&gt;"",VLOOKUP(J16,Tabla1[#All],4,FALSE),"")</f>
@@ -2773,11 +3104,11 @@
       </c>
       <c r="AB16" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>['OAT','left','Outdoor-Air Temp (temp)','smoothedLine']</v>
+        <v>['OAT','left','Common zone','Outdoor-Air Temp (temp)']</v>
       </c>
       <c r="AC16" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>,['OADPS','right','Outdoor-Air Damper Position Signal (%)','column']</v>
+        <v>,['OADPS','right','Air handle unit','Outdoor-Air Damper Position Signal (%)']</v>
       </c>
       <c r="AD16" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2798,7 +3129,7 @@
       </c>
       <c r="B17" t="str">
         <f t="shared" si="0"/>
-        <v>if ($('#dparameters').html().trim()==7) { var dataparameter=[['CCV','right','Cooling-Coil Valve Signal (%)','column'],['DATSP','left','Discharge-Air Temp Set Point','smoothedLine'],['OADPS','right','Outdoor-Air Damper Position Signal (%)','column'],['OAT','left','Outdoor-Air Temp (temp)','smoothedLine']]; }</v>
+        <v>if ($('#dparameters').html().trim()==7) { var dataparameter=[['CCV','right','Chiller','Cooling-Coil Valve Signal (%)'],['DATSP','left','Air handle unit','Discharge-Air Temp Set Point'],['OADPS','right','Air handle unit','Outdoor-Air Damper Position Signal (%)'],['OAT','left','Common zone','Outdoor-Air Temp (temp)']]; }</v>
       </c>
       <c r="H17" t="s">
         <v>12</v>
@@ -2834,19 +3165,19 @@
       </c>
       <c r="R17" s="4" t="str">
         <f>IF(H17&lt;&gt;"",VLOOKUP(H17,Tabla1[#All],3,FALSE),"")</f>
-        <v>Cooling-Coil Valve Signal (%)</v>
+        <v>Chiller</v>
       </c>
       <c r="S17" s="4" t="str">
         <f>IF(I17&lt;&gt;"",VLOOKUP(I17,Tabla1[#All],3,FALSE),"")</f>
-        <v>Discharge-Air Temp Set Point</v>
+        <v>Air handle unit</v>
       </c>
       <c r="T17" s="4" t="str">
         <f>IF(J17&lt;&gt;"",VLOOKUP(J17,Tabla1[#All],3,FALSE),"")</f>
-        <v>Outdoor-Air Damper Position Signal (%)</v>
+        <v>Air handle unit</v>
       </c>
       <c r="U17" s="4" t="str">
         <f>IF(K17&lt;&gt;"",VLOOKUP(K17,Tabla1[#All],3,FALSE),"")</f>
-        <v>Outdoor-Air Temp (temp)</v>
+        <v>Common zone</v>
       </c>
       <c r="V17" s="4" t="str">
         <f>IF(L17&lt;&gt;"",VLOOKUP(L17,Tabla1[#All],3,FALSE),"")</f>
@@ -2854,19 +3185,19 @@
       </c>
       <c r="W17" s="1" t="str">
         <f>IF(H17&lt;&gt;"",VLOOKUP(H17,Tabla1[#All],4,FALSE),"")</f>
-        <v>column</v>
+        <v>Cooling-Coil Valve Signal (%)</v>
       </c>
       <c r="X17" s="1" t="str">
         <f>IF(I17&lt;&gt;"",VLOOKUP(I17,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Discharge-Air Temp Set Point</v>
       </c>
       <c r="Y17" s="1" t="str">
         <f>IF(J17&lt;&gt;"",VLOOKUP(J17,Tabla1[#All],4,FALSE),"")</f>
-        <v>column</v>
+        <v>Outdoor-Air Damper Position Signal (%)</v>
       </c>
       <c r="Z17" s="1" t="str">
         <f>IF(K17&lt;&gt;"",VLOOKUP(K17,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Outdoor-Air Temp (temp)</v>
       </c>
       <c r="AA17" s="1" t="str">
         <f>IF(L17&lt;&gt;"",VLOOKUP(L17,Tabla1[#All],4,FALSE),"")</f>
@@ -2874,19 +3205,19 @@
       </c>
       <c r="AB17" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>['CCV','right','Cooling-Coil Valve Signal (%)','column']</v>
+        <v>['CCV','right','Chiller','Cooling-Coil Valve Signal (%)']</v>
       </c>
       <c r="AC17" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>,['DATSP','left','Discharge-Air Temp Set Point','smoothedLine']</v>
+        <v>,['DATSP','left','Air handle unit','Discharge-Air Temp Set Point']</v>
       </c>
       <c r="AD17" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>,['OADPS','right','Outdoor-Air Damper Position Signal (%)','column']</v>
+        <v>,['OADPS','right','Air handle unit','Outdoor-Air Damper Position Signal (%)']</v>
       </c>
       <c r="AE17" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>,['OAT','left','Outdoor-Air Temp (temp)','smoothedLine']</v>
+        <v>,['OAT','left','Common zone','Outdoor-Air Temp (temp)']</v>
       </c>
       <c r="AF17" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2899,7 +3230,7 @@
       </c>
       <c r="B18" t="str">
         <f t="shared" si="0"/>
-        <v>if ($('#dparameters').html().trim()==8) { var dataparameter=[['CCV','right','Cooling-Coil Valve Signal (%)','column'],['OADPS','right','Outdoor-Air Damper Position Signal (%)','column'],['OAT','left','Outdoor-Air Temp (temp)','smoothedLine']]; }</v>
+        <v>if ($('#dparameters').html().trim()==8) { var dataparameter=[['CCV','right','Chiller','Cooling-Coil Valve Signal (%)'],['OADPS','right','Air handle unit','Outdoor-Air Damper Position Signal (%)'],['OAT','left','Common zone','Outdoor-Air Temp (temp)']]; }</v>
       </c>
       <c r="H18" t="s">
         <v>12</v>
@@ -2932,15 +3263,15 @@
       </c>
       <c r="R18" s="4" t="str">
         <f>IF(H18&lt;&gt;"",VLOOKUP(H18,Tabla1[#All],3,FALSE),"")</f>
-        <v>Cooling-Coil Valve Signal (%)</v>
+        <v>Chiller</v>
       </c>
       <c r="S18" s="4" t="str">
         <f>IF(I18&lt;&gt;"",VLOOKUP(I18,Tabla1[#All],3,FALSE),"")</f>
-        <v>Outdoor-Air Damper Position Signal (%)</v>
+        <v>Air handle unit</v>
       </c>
       <c r="T18" s="4" t="str">
         <f>IF(J18&lt;&gt;"",VLOOKUP(J18,Tabla1[#All],3,FALSE),"")</f>
-        <v>Outdoor-Air Temp (temp)</v>
+        <v>Common zone</v>
       </c>
       <c r="U18" s="4" t="str">
         <f>IF(K18&lt;&gt;"",VLOOKUP(K18,Tabla1[#All],3,FALSE),"")</f>
@@ -2952,15 +3283,15 @@
       </c>
       <c r="W18" s="1" t="str">
         <f>IF(H18&lt;&gt;"",VLOOKUP(H18,Tabla1[#All],4,FALSE),"")</f>
-        <v>column</v>
+        <v>Cooling-Coil Valve Signal (%)</v>
       </c>
       <c r="X18" s="1" t="str">
         <f>IF(I18&lt;&gt;"",VLOOKUP(I18,Tabla1[#All],4,FALSE),"")</f>
-        <v>column</v>
+        <v>Outdoor-Air Damper Position Signal (%)</v>
       </c>
       <c r="Y18" s="1" t="str">
         <f>IF(J18&lt;&gt;"",VLOOKUP(J18,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Outdoor-Air Temp (temp)</v>
       </c>
       <c r="Z18" s="1" t="str">
         <f>IF(K18&lt;&gt;"",VLOOKUP(K18,Tabla1[#All],4,FALSE),"")</f>
@@ -2972,15 +3303,15 @@
       </c>
       <c r="AB18" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>['CCV','right','Cooling-Coil Valve Signal (%)','column']</v>
+        <v>['CCV','right','Chiller','Cooling-Coil Valve Signal (%)']</v>
       </c>
       <c r="AC18" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>,['OADPS','right','Outdoor-Air Damper Position Signal (%)','column']</v>
+        <v>,['OADPS','right','Air handle unit','Outdoor-Air Damper Position Signal (%)']</v>
       </c>
       <c r="AD18" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>,['OAT','left','Outdoor-Air Temp (temp)','smoothedLine']</v>
+        <v>,['OAT','left','Common zone','Outdoor-Air Temp (temp)']</v>
       </c>
       <c r="AE18" s="3" t="str">
         <f t="shared" si="2"/>
@@ -2997,7 +3328,7 @@
       </c>
       <c r="B19" t="str">
         <f t="shared" si="0"/>
-        <v>if ($('#dparameters').html().trim()==9) { var dataparameter=[['CCV','right','Cooling-Coil Valve Signal (%)','column'],['OADPS','right','Outdoor-Air Damper Position Signal (%)','column']]; }</v>
+        <v>if ($('#dparameters').html().trim()==9) { var dataparameter=[['CCV','right','Chiller','Cooling-Coil Valve Signal (%)'],['OADPS','right','Air handle unit','Outdoor-Air Damper Position Signal (%)']]; }</v>
       </c>
       <c r="H19" t="s">
         <v>12</v>
@@ -3027,11 +3358,11 @@
       </c>
       <c r="R19" s="4" t="str">
         <f>IF(H19&lt;&gt;"",VLOOKUP(H19,Tabla1[#All],3,FALSE),"")</f>
-        <v>Cooling-Coil Valve Signal (%)</v>
+        <v>Chiller</v>
       </c>
       <c r="S19" s="4" t="str">
         <f>IF(I19&lt;&gt;"",VLOOKUP(I19,Tabla1[#All],3,FALSE),"")</f>
-        <v>Outdoor-Air Damper Position Signal (%)</v>
+        <v>Air handle unit</v>
       </c>
       <c r="T19" s="4" t="str">
         <f>IF(J19&lt;&gt;"",VLOOKUP(J19,Tabla1[#All],3,FALSE),"")</f>
@@ -3047,11 +3378,11 @@
       </c>
       <c r="W19" s="1" t="str">
         <f>IF(H19&lt;&gt;"",VLOOKUP(H19,Tabla1[#All],4,FALSE),"")</f>
-        <v>column</v>
+        <v>Cooling-Coil Valve Signal (%)</v>
       </c>
       <c r="X19" s="1" t="str">
         <f>IF(I19&lt;&gt;"",VLOOKUP(I19,Tabla1[#All],4,FALSE),"")</f>
-        <v>column</v>
+        <v>Outdoor-Air Damper Position Signal (%)</v>
       </c>
       <c r="Y19" s="1" t="str">
         <f>IF(J19&lt;&gt;"",VLOOKUP(J19,Tabla1[#All],4,FALSE),"")</f>
@@ -3067,11 +3398,11 @@
       </c>
       <c r="AB19" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>['CCV','right','Cooling-Coil Valve Signal (%)','column']</v>
+        <v>['CCV','right','Chiller','Cooling-Coil Valve Signal (%)']</v>
       </c>
       <c r="AC19" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>,['OADPS','right','Outdoor-Air Damper Position Signal (%)','column']</v>
+        <v>,['OADPS','right','Air handle unit','Outdoor-Air Damper Position Signal (%)']</v>
       </c>
       <c r="AD19" s="3" t="str">
         <f t="shared" si="2"/>
@@ -3092,7 +3423,7 @@
       </c>
       <c r="B20" t="str">
         <f t="shared" si="0"/>
-        <v>if ($('#dparameters').html().trim()==10) { var dataparameter=[['DAT','left','Discharge-Air Temp','smoothedLine'],['MAT','left','Mixed-Air Temp','smoothedLine'],['OAT','left','Outdoor-Air Temp (temp)','smoothedLine'],['RAT','left','Return-Air Temp','smoothedLine']]; }</v>
+        <v>if ($('#dparameters').html().trim()==10) { var dataparameter=[['DAT','left','Air handle unit','Discharge-Air Temp'],['MAT','left','Air handle unit','Mixed-Air Temp'],['OAT','left','Common zone','Outdoor-Air Temp (temp)'],['RAT','left','Air handle unit','Return-Air Temp']]; }</v>
       </c>
       <c r="H20" t="s">
         <v>13</v>
@@ -3128,19 +3459,19 @@
       </c>
       <c r="R20" s="4" t="str">
         <f>IF(H20&lt;&gt;"",VLOOKUP(H20,Tabla1[#All],3,FALSE),"")</f>
-        <v>Discharge-Air Temp</v>
+        <v>Air handle unit</v>
       </c>
       <c r="S20" s="4" t="str">
         <f>IF(I20&lt;&gt;"",VLOOKUP(I20,Tabla1[#All],3,FALSE),"")</f>
-        <v>Mixed-Air Temp</v>
+        <v>Air handle unit</v>
       </c>
       <c r="T20" s="4" t="str">
         <f>IF(J20&lt;&gt;"",VLOOKUP(J20,Tabla1[#All],3,FALSE),"")</f>
-        <v>Outdoor-Air Temp (temp)</v>
+        <v>Common zone</v>
       </c>
       <c r="U20" s="4" t="str">
         <f>IF(K20&lt;&gt;"",VLOOKUP(K20,Tabla1[#All],3,FALSE),"")</f>
-        <v>Return-Air Temp</v>
+        <v>Air handle unit</v>
       </c>
       <c r="V20" s="4" t="str">
         <f>IF(L20&lt;&gt;"",VLOOKUP(L20,Tabla1[#All],3,FALSE),"")</f>
@@ -3148,19 +3479,19 @@
       </c>
       <c r="W20" s="1" t="str">
         <f>IF(H20&lt;&gt;"",VLOOKUP(H20,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Discharge-Air Temp</v>
       </c>
       <c r="X20" s="1" t="str">
         <f>IF(I20&lt;&gt;"",VLOOKUP(I20,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Mixed-Air Temp</v>
       </c>
       <c r="Y20" s="1" t="str">
         <f>IF(J20&lt;&gt;"",VLOOKUP(J20,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Outdoor-Air Temp (temp)</v>
       </c>
       <c r="Z20" s="1" t="str">
         <f>IF(K20&lt;&gt;"",VLOOKUP(K20,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Return-Air Temp</v>
       </c>
       <c r="AA20" s="1" t="str">
         <f>IF(L20&lt;&gt;"",VLOOKUP(L20,Tabla1[#All],4,FALSE),"")</f>
@@ -3168,19 +3499,19 @@
       </c>
       <c r="AB20" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>['DAT','left','Discharge-Air Temp','smoothedLine']</v>
+        <v>['DAT','left','Air handle unit','Discharge-Air Temp']</v>
       </c>
       <c r="AC20" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>,['MAT','left','Mixed-Air Temp','smoothedLine']</v>
+        <v>,['MAT','left','Air handle unit','Mixed-Air Temp']</v>
       </c>
       <c r="AD20" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>,['OAT','left','Outdoor-Air Temp (temp)','smoothedLine']</v>
+        <v>,['OAT','left','Common zone','Outdoor-Air Temp (temp)']</v>
       </c>
       <c r="AE20" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>,['RAT','left','Return-Air Temp','smoothedLine']</v>
+        <v>,['RAT','left','Air handle unit','Return-Air Temp']</v>
       </c>
       <c r="AF20" s="3" t="str">
         <f t="shared" si="2"/>
@@ -3193,7 +3524,7 @@
       </c>
       <c r="B21" t="str">
         <f t="shared" si="0"/>
-        <v>if ($('#dparameters').html().trim()==11) { var dataparameter=[['CCV','right','Cooling-Coil Valve Signal (%)','column'],['HCVS','right','Heating-Coil Valve Signal (%)','column'],['OAT','left','Outdoor-Air Temp (temp)','smoothedLine']]; }</v>
+        <v>if ($('#dparameters').html().trim()==11) { var dataparameter=[['CCV','right','Chiller','Cooling-Coil Valve Signal (%)'],['HCVS','right','Boiler','Heating-Coil Valve Signal (%)'],['OAT','left','Common zone','Outdoor-Air Temp (temp)']]; }</v>
       </c>
       <c r="H21" t="s">
         <v>12</v>
@@ -3226,15 +3557,15 @@
       </c>
       <c r="R21" s="4" t="str">
         <f>IF(H21&lt;&gt;"",VLOOKUP(H21,Tabla1[#All],3,FALSE),"")</f>
-        <v>Cooling-Coil Valve Signal (%)</v>
+        <v>Chiller</v>
       </c>
       <c r="S21" s="4" t="str">
         <f>IF(I21&lt;&gt;"",VLOOKUP(I21,Tabla1[#All],3,FALSE),"")</f>
-        <v>Heating-Coil Valve Signal (%)</v>
+        <v>Boiler</v>
       </c>
       <c r="T21" s="4" t="str">
         <f>IF(J21&lt;&gt;"",VLOOKUP(J21,Tabla1[#All],3,FALSE),"")</f>
-        <v>Outdoor-Air Temp (temp)</v>
+        <v>Common zone</v>
       </c>
       <c r="U21" s="4" t="str">
         <f>IF(K21&lt;&gt;"",VLOOKUP(K21,Tabla1[#All],3,FALSE),"")</f>
@@ -3246,15 +3577,15 @@
       </c>
       <c r="W21" s="1" t="str">
         <f>IF(H21&lt;&gt;"",VLOOKUP(H21,Tabla1[#All],4,FALSE),"")</f>
-        <v>column</v>
+        <v>Cooling-Coil Valve Signal (%)</v>
       </c>
       <c r="X21" s="1" t="str">
         <f>IF(I21&lt;&gt;"",VLOOKUP(I21,Tabla1[#All],4,FALSE),"")</f>
-        <v>column</v>
+        <v>Heating-Coil Valve Signal (%)</v>
       </c>
       <c r="Y21" s="1" t="str">
         <f>IF(J21&lt;&gt;"",VLOOKUP(J21,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Outdoor-Air Temp (temp)</v>
       </c>
       <c r="Z21" s="1" t="str">
         <f>IF(K21&lt;&gt;"",VLOOKUP(K21,Tabla1[#All],4,FALSE),"")</f>
@@ -3266,15 +3597,15 @@
       </c>
       <c r="AB21" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>['CCV','right','Cooling-Coil Valve Signal (%)','column']</v>
+        <v>['CCV','right','Chiller','Cooling-Coil Valve Signal (%)']</v>
       </c>
       <c r="AC21" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>,['HCVS','right','Heating-Coil Valve Signal (%)','column']</v>
+        <v>,['HCVS','right','Boiler','Heating-Coil Valve Signal (%)']</v>
       </c>
       <c r="AD21" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>,['OAT','left','Outdoor-Air Temp (temp)','smoothedLine']</v>
+        <v>,['OAT','left','Common zone','Outdoor-Air Temp (temp)']</v>
       </c>
       <c r="AE21" s="3" t="str">
         <f t="shared" si="2"/>
@@ -3291,7 +3622,7 @@
       </c>
       <c r="B22" t="str">
         <f t="shared" si="0"/>
-        <v>if ($('#dparameters').html().trim()==12) { var dataparameter=[['ChWST','left','Chilled-Water Supply Temp','smoothedLine'],['OAT','left','Outdoor-Air Temp (temp)','smoothedLine']]; }</v>
+        <v>if ($('#dparameters').html().trim()==12) { var dataparameter=[['ChWST','left','Chiller','Chilled-Water Supply Temp'],['OAT','left','Common zone','Outdoor-Air Temp (temp)']]; }</v>
       </c>
       <c r="H22" t="s">
         <v>14</v>
@@ -3321,11 +3652,11 @@
       </c>
       <c r="R22" s="4" t="str">
         <f>IF(H22&lt;&gt;"",VLOOKUP(H22,Tabla1[#All],3,FALSE),"")</f>
-        <v>Chilled-Water Supply Temp</v>
+        <v>Chiller</v>
       </c>
       <c r="S22" s="4" t="str">
         <f>IF(I22&lt;&gt;"",VLOOKUP(I22,Tabla1[#All],3,FALSE),"")</f>
-        <v>Outdoor-Air Temp (temp)</v>
+        <v>Common zone</v>
       </c>
       <c r="T22" s="4" t="str">
         <f>IF(J22&lt;&gt;"",VLOOKUP(J22,Tabla1[#All],3,FALSE),"")</f>
@@ -3341,11 +3672,11 @@
       </c>
       <c r="W22" s="1" t="str">
         <f>IF(H22&lt;&gt;"",VLOOKUP(H22,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Chilled-Water Supply Temp</v>
       </c>
       <c r="X22" s="1" t="str">
         <f>IF(I22&lt;&gt;"",VLOOKUP(I22,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Outdoor-Air Temp (temp)</v>
       </c>
       <c r="Y22" s="1" t="str">
         <f>IF(J22&lt;&gt;"",VLOOKUP(J22,Tabla1[#All],4,FALSE),"")</f>
@@ -3361,11 +3692,11 @@
       </c>
       <c r="AB22" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>['ChWST','left','Chilled-Water Supply Temp','smoothedLine']</v>
+        <v>['ChWST','left','Chiller','Chilled-Water Supply Temp']</v>
       </c>
       <c r="AC22" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>,['OAT','left','Outdoor-Air Temp (temp)','smoothedLine']</v>
+        <v>,['OAT','left','Common zone','Outdoor-Air Temp (temp)']</v>
       </c>
       <c r="AD22" s="3" t="str">
         <f t="shared" si="2"/>
@@ -3386,7 +3717,7 @@
       </c>
       <c r="B23" t="str">
         <f t="shared" si="0"/>
-        <v>if ($('#dparameters').html().trim()==13) { var dataparameter=[['ChWST','left','Chilled-Water Supply Temp','smoothedLine'],['CCV','right','Cooling-Coil Valve Signal (%)','column'],['OAT','left','Outdoor-Air Temp (temp)','smoothedLine']]; }</v>
+        <v>if ($('#dparameters').html().trim()==13) { var dataparameter=[['ChWST','left','Chiller','Chilled-Water Supply Temp'],['CCV','right','Chiller','Cooling-Coil Valve Signal (%)'],['OAT','left','Common zone','Outdoor-Air Temp (temp)']]; }</v>
       </c>
       <c r="H23" t="s">
         <v>14</v>
@@ -3419,15 +3750,15 @@
       </c>
       <c r="R23" s="4" t="str">
         <f>IF(H23&lt;&gt;"",VLOOKUP(H23,Tabla1[#All],3,FALSE),"")</f>
-        <v>Chilled-Water Supply Temp</v>
+        <v>Chiller</v>
       </c>
       <c r="S23" s="4" t="str">
         <f>IF(I23&lt;&gt;"",VLOOKUP(I23,Tabla1[#All],3,FALSE),"")</f>
-        <v>Cooling-Coil Valve Signal (%)</v>
+        <v>Chiller</v>
       </c>
       <c r="T23" s="4" t="str">
         <f>IF(J23&lt;&gt;"",VLOOKUP(J23,Tabla1[#All],3,FALSE),"")</f>
-        <v>Outdoor-Air Temp (temp)</v>
+        <v>Common zone</v>
       </c>
       <c r="U23" s="4" t="str">
         <f>IF(K23&lt;&gt;"",VLOOKUP(K23,Tabla1[#All],3,FALSE),"")</f>
@@ -3439,15 +3770,15 @@
       </c>
       <c r="W23" s="1" t="str">
         <f>IF(H23&lt;&gt;"",VLOOKUP(H23,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Chilled-Water Supply Temp</v>
       </c>
       <c r="X23" s="1" t="str">
         <f>IF(I23&lt;&gt;"",VLOOKUP(I23,Tabla1[#All],4,FALSE),"")</f>
-        <v>column</v>
+        <v>Cooling-Coil Valve Signal (%)</v>
       </c>
       <c r="Y23" s="1" t="str">
         <f>IF(J23&lt;&gt;"",VLOOKUP(J23,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Outdoor-Air Temp (temp)</v>
       </c>
       <c r="Z23" s="1" t="str">
         <f>IF(K23&lt;&gt;"",VLOOKUP(K23,Tabla1[#All],4,FALSE),"")</f>
@@ -3459,15 +3790,15 @@
       </c>
       <c r="AB23" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>['ChWST','left','Chilled-Water Supply Temp','smoothedLine']</v>
+        <v>['ChWST','left','Chiller','Chilled-Water Supply Temp']</v>
       </c>
       <c r="AC23" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>,['CCV','right','Cooling-Coil Valve Signal (%)','column']</v>
+        <v>,['CCV','right','Chiller','Cooling-Coil Valve Signal (%)']</v>
       </c>
       <c r="AD23" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>,['OAT','left','Outdoor-Air Temp (temp)','smoothedLine']</v>
+        <v>,['OAT','left','Common zone','Outdoor-Air Temp (temp)']</v>
       </c>
       <c r="AE23" s="3" t="str">
         <f t="shared" si="2"/>
@@ -3484,7 +3815,7 @@
       </c>
       <c r="B24" t="str">
         <f t="shared" si="0"/>
-        <v>if ($('#dparameters').html().trim()==14) { var dataparameter=[['ChWRT','left','Chilled-Water Return Temp','smoothedLine'],['ChWST','left','Chilled-Water Supply Temp','smoothedLine'],['OAT','left','Outdoor-Air Temp (temp)','smoothedLine']]; }</v>
+        <v>if ($('#dparameters').html().trim()==14) { var dataparameter=[['ChWRT','left','Chiller','Chilled-Water Return Temp'],['ChWST','left','Chiller','Chilled-Water Supply Temp'],['OAT','left','Common zone','Outdoor-Air Temp (temp)']]; }</v>
       </c>
       <c r="H24" t="s">
         <v>15</v>
@@ -3517,15 +3848,15 @@
       </c>
       <c r="R24" s="4" t="str">
         <f>IF(H24&lt;&gt;"",VLOOKUP(H24,Tabla1[#All],3,FALSE),"")</f>
-        <v>Chilled-Water Return Temp</v>
+        <v>Chiller</v>
       </c>
       <c r="S24" s="4" t="str">
         <f>IF(I24&lt;&gt;"",VLOOKUP(I24,Tabla1[#All],3,FALSE),"")</f>
-        <v>Chilled-Water Supply Temp</v>
+        <v>Chiller</v>
       </c>
       <c r="T24" s="4" t="str">
         <f>IF(J24&lt;&gt;"",VLOOKUP(J24,Tabla1[#All],3,FALSE),"")</f>
-        <v>Outdoor-Air Temp (temp)</v>
+        <v>Common zone</v>
       </c>
       <c r="U24" s="4" t="str">
         <f>IF(K24&lt;&gt;"",VLOOKUP(K24,Tabla1[#All],3,FALSE),"")</f>
@@ -3537,15 +3868,15 @@
       </c>
       <c r="W24" s="1" t="str">
         <f>IF(H24&lt;&gt;"",VLOOKUP(H24,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Chilled-Water Return Temp</v>
       </c>
       <c r="X24" s="1" t="str">
         <f>IF(I24&lt;&gt;"",VLOOKUP(I24,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Chilled-Water Supply Temp</v>
       </c>
       <c r="Y24" s="1" t="str">
         <f>IF(J24&lt;&gt;"",VLOOKUP(J24,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Outdoor-Air Temp (temp)</v>
       </c>
       <c r="Z24" s="1" t="str">
         <f>IF(K24&lt;&gt;"",VLOOKUP(K24,Tabla1[#All],4,FALSE),"")</f>
@@ -3557,15 +3888,15 @@
       </c>
       <c r="AB24" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>['ChWRT','left','Chilled-Water Return Temp','smoothedLine']</v>
+        <v>['ChWRT','left','Chiller','Chilled-Water Return Temp']</v>
       </c>
       <c r="AC24" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>,['ChWST','left','Chilled-Water Supply Temp','smoothedLine']</v>
+        <v>,['ChWST','left','Chiller','Chilled-Water Supply Temp']</v>
       </c>
       <c r="AD24" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>,['OAT','left','Outdoor-Air Temp (temp)','smoothedLine']</v>
+        <v>,['OAT','left','Common zone','Outdoor-Air Temp (temp)']</v>
       </c>
       <c r="AE24" s="3" t="str">
         <f t="shared" si="2"/>
@@ -3582,7 +3913,7 @@
       </c>
       <c r="B25" t="str">
         <f t="shared" si="0"/>
-        <v>if ($('#dparameters').html().trim()==15) { var dataparameter=[['CHWRT','left','Chilled-Water Return Temp','smoothedLine'],['CCV','right','Cooling-Coil Valve Signal (%)','column']]; }</v>
+        <v>if ($('#dparameters').html().trim()==15) { var dataparameter=[['CHWRT','left','Chiller','Chilled-Water Return Temp'],['CCV','right','Chiller','Cooling-Coil Valve Signal (%)']]; }</v>
       </c>
       <c r="H25" t="s">
         <v>16</v>
@@ -3612,11 +3943,11 @@
       </c>
       <c r="R25" s="4" t="str">
         <f>IF(H25&lt;&gt;"",VLOOKUP(H25,Tabla1[#All],3,FALSE),"")</f>
-        <v>Chilled-Water Return Temp</v>
+        <v>Chiller</v>
       </c>
       <c r="S25" s="4" t="str">
         <f>IF(I25&lt;&gt;"",VLOOKUP(I25,Tabla1[#All],3,FALSE),"")</f>
-        <v>Cooling-Coil Valve Signal (%)</v>
+        <v>Chiller</v>
       </c>
       <c r="T25" s="4" t="str">
         <f>IF(J25&lt;&gt;"",VLOOKUP(J25,Tabla1[#All],3,FALSE),"")</f>
@@ -3632,11 +3963,11 @@
       </c>
       <c r="W25" s="1" t="str">
         <f>IF(H25&lt;&gt;"",VLOOKUP(H25,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Chilled-Water Return Temp</v>
       </c>
       <c r="X25" s="1" t="str">
         <f>IF(I25&lt;&gt;"",VLOOKUP(I25,Tabla1[#All],4,FALSE),"")</f>
-        <v>column</v>
+        <v>Cooling-Coil Valve Signal (%)</v>
       </c>
       <c r="Y25" s="1" t="str">
         <f>IF(J25&lt;&gt;"",VLOOKUP(J25,Tabla1[#All],4,FALSE),"")</f>
@@ -3652,11 +3983,11 @@
       </c>
       <c r="AB25" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>['CHWRT','left','Chilled-Water Return Temp','smoothedLine']</v>
+        <v>['CHWRT','left','Chiller','Chilled-Water Return Temp']</v>
       </c>
       <c r="AC25" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>,['CCV','right','Cooling-Coil Valve Signal (%)','column']</v>
+        <v>,['CCV','right','Chiller','Cooling-Coil Valve Signal (%)']</v>
       </c>
       <c r="AD25" s="3" t="str">
         <f t="shared" si="2"/>
@@ -3677,7 +4008,7 @@
       </c>
       <c r="B26" t="str">
         <f t="shared" si="0"/>
-        <v>if ($('#dparameters').html().trim()==16) { var dataparameter=[['HWST','left','Hot-Water Supply Temp','smoothedLine'],['OAT','left','Outdoor-Air Temp (temp)','smoothedLine']]; }</v>
+        <v>if ($('#dparameters').html().trim()==16) { var dataparameter=[['HWST','left','Boiler','Hot-Water Supply Temp'],['OAT','left','Common zone','Outdoor-Air Temp (temp)']]; }</v>
       </c>
       <c r="H26" t="s">
         <v>17</v>
@@ -3707,11 +4038,11 @@
       </c>
       <c r="R26" s="4" t="str">
         <f>IF(H26&lt;&gt;"",VLOOKUP(H26,Tabla1[#All],3,FALSE),"")</f>
-        <v>Hot-Water Supply Temp</v>
+        <v>Boiler</v>
       </c>
       <c r="S26" s="4" t="str">
         <f>IF(I26&lt;&gt;"",VLOOKUP(I26,Tabla1[#All],3,FALSE),"")</f>
-        <v>Outdoor-Air Temp (temp)</v>
+        <v>Common zone</v>
       </c>
       <c r="T26" s="4" t="str">
         <f>IF(J26&lt;&gt;"",VLOOKUP(J26,Tabla1[#All],3,FALSE),"")</f>
@@ -3727,11 +4058,11 @@
       </c>
       <c r="W26" s="1" t="str">
         <f>IF(H26&lt;&gt;"",VLOOKUP(H26,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Hot-Water Supply Temp</v>
       </c>
       <c r="X26" s="1" t="str">
         <f>IF(I26&lt;&gt;"",VLOOKUP(I26,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Outdoor-Air Temp (temp)</v>
       </c>
       <c r="Y26" s="1" t="str">
         <f>IF(J26&lt;&gt;"",VLOOKUP(J26,Tabla1[#All],4,FALSE),"")</f>
@@ -3747,11 +4078,11 @@
       </c>
       <c r="AB26" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>['HWST','left','Hot-Water Supply Temp','smoothedLine']</v>
+        <v>['HWST','left','Boiler','Hot-Water Supply Temp']</v>
       </c>
       <c r="AC26" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>,['OAT','left','Outdoor-Air Temp (temp)','smoothedLine']</v>
+        <v>,['OAT','left','Common zone','Outdoor-Air Temp (temp)']</v>
       </c>
       <c r="AD26" s="3" t="str">
         <f t="shared" si="2"/>
@@ -3772,7 +4103,7 @@
       </c>
       <c r="B27" t="str">
         <f t="shared" si="0"/>
-        <v>if ($('#dparameters').html().trim()==17) { var dataparameter=[['HWRT','left','Hot-Water Return Temp','smoothedLine'],['HWST','left','Hot-Water Supply Temp','smoothedLine'],['OAT','left','Outdoor-Air Temp (temp)','smoothedLine']]; }</v>
+        <v>if ($('#dparameters').html().trim()==17) { var dataparameter=[['HWRT','left','Boiler','Hot-Water Return Temp'],['HWST','left','Boiler','Hot-Water Supply Temp'],['OAT','left','Common zone','Outdoor-Air Temp (temp)']]; }</v>
       </c>
       <c r="H27" t="s">
         <v>18</v>
@@ -3805,15 +4136,15 @@
       </c>
       <c r="R27" s="4" t="str">
         <f>IF(H27&lt;&gt;"",VLOOKUP(H27,Tabla1[#All],3,FALSE),"")</f>
-        <v>Hot-Water Return Temp</v>
+        <v>Boiler</v>
       </c>
       <c r="S27" s="4" t="str">
         <f>IF(I27&lt;&gt;"",VLOOKUP(I27,Tabla1[#All],3,FALSE),"")</f>
-        <v>Hot-Water Supply Temp</v>
+        <v>Boiler</v>
       </c>
       <c r="T27" s="4" t="str">
         <f>IF(J27&lt;&gt;"",VLOOKUP(J27,Tabla1[#All],3,FALSE),"")</f>
-        <v>Outdoor-Air Temp (temp)</v>
+        <v>Common zone</v>
       </c>
       <c r="U27" s="4" t="str">
         <f>IF(K27&lt;&gt;"",VLOOKUP(K27,Tabla1[#All],3,FALSE),"")</f>
@@ -3825,15 +4156,15 @@
       </c>
       <c r="W27" s="1" t="str">
         <f>IF(H27&lt;&gt;"",VLOOKUP(H27,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Hot-Water Return Temp</v>
       </c>
       <c r="X27" s="1" t="str">
         <f>IF(I27&lt;&gt;"",VLOOKUP(I27,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Hot-Water Supply Temp</v>
       </c>
       <c r="Y27" s="1" t="str">
         <f>IF(J27&lt;&gt;"",VLOOKUP(J27,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Outdoor-Air Temp (temp)</v>
       </c>
       <c r="Z27" s="1" t="str">
         <f>IF(K27&lt;&gt;"",VLOOKUP(K27,Tabla1[#All],4,FALSE),"")</f>
@@ -3845,15 +4176,15 @@
       </c>
       <c r="AB27" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>['HWRT','left','Hot-Water Return Temp','smoothedLine']</v>
+        <v>['HWRT','left','Boiler','Hot-Water Return Temp']</v>
       </c>
       <c r="AC27" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>,['HWST','left','Hot-Water Supply Temp','smoothedLine']</v>
+        <v>,['HWST','left','Boiler','Hot-Water Supply Temp']</v>
       </c>
       <c r="AD27" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>,['OAT','left','Outdoor-Air Temp (temp)','smoothedLine']</v>
+        <v>,['OAT','left','Common zone','Outdoor-Air Temp (temp)']</v>
       </c>
       <c r="AE27" s="3" t="str">
         <f t="shared" si="2"/>
@@ -3870,7 +4201,7 @@
       </c>
       <c r="B28" t="str">
         <f t="shared" si="0"/>
-        <v>if ($('#dparameters').html().trim()==18) { var dataparameter=[['HWLDP','left','Hot-Water Loop Differential Pressure','smoothedLine'],['HCVS','right','Heating-Coil Valve Signal (%)','column']]; }</v>
+        <v>if ($('#dparameters').html().trim()==18) { var dataparameter=[['HWLDP','left','Boiler','Hot-Water Loop Differential Pressure'],['HCVS','right','Boiler','Heating-Coil Valve Signal (%)']]; }</v>
       </c>
       <c r="H28" t="s">
         <v>19</v>
@@ -3900,11 +4231,11 @@
       </c>
       <c r="R28" s="4" t="str">
         <f>IF(H28&lt;&gt;"",VLOOKUP(H28,Tabla1[#All],3,FALSE),"")</f>
-        <v>Hot-Water Loop Differential Pressure</v>
+        <v>Boiler</v>
       </c>
       <c r="S28" s="4" t="str">
         <f>IF(I28&lt;&gt;"",VLOOKUP(I28,Tabla1[#All],3,FALSE),"")</f>
-        <v>Heating-Coil Valve Signal (%)</v>
+        <v>Boiler</v>
       </c>
       <c r="T28" s="4" t="str">
         <f>IF(J28&lt;&gt;"",VLOOKUP(J28,Tabla1[#All],3,FALSE),"")</f>
@@ -3920,11 +4251,11 @@
       </c>
       <c r="W28" s="1" t="str">
         <f>IF(H28&lt;&gt;"",VLOOKUP(H28,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Hot-Water Loop Differential Pressure</v>
       </c>
       <c r="X28" s="1" t="str">
         <f>IF(I28&lt;&gt;"",VLOOKUP(I28,Tabla1[#All],4,FALSE),"")</f>
-        <v>column</v>
+        <v>Heating-Coil Valve Signal (%)</v>
       </c>
       <c r="Y28" s="1" t="str">
         <f>IF(J28&lt;&gt;"",VLOOKUP(J28,Tabla1[#All],4,FALSE),"")</f>
@@ -3940,11 +4271,11 @@
       </c>
       <c r="AB28" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>['HWLDP','left','Hot-Water Loop Differential Pressure','smoothedLine']</v>
+        <v>['HWLDP','left','Boiler','Hot-Water Loop Differential Pressure']</v>
       </c>
       <c r="AC28" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>,['HCVS','right','Heating-Coil Valve Signal (%)','column']</v>
+        <v>,['HCVS','right','Boiler','Heating-Coil Valve Signal (%)']</v>
       </c>
       <c r="AD28" s="3" t="str">
         <f t="shared" si="2"/>
@@ -3965,7 +4296,7 @@
       </c>
       <c r="B29" t="str">
         <f t="shared" si="0"/>
-        <v>if ($('#dparameters').html().trim()==19) { var dataparameter=[['OAT','left','Outdoor-Air Temp (temp)','smoothedLine'],['OADPS','right','Outdoor-Air Damper Position Signal (%)','column'],['OAF','right','Outdoor-Air Fraction temp','column'],['OM','right','Occupancy Mode','column']]; }</v>
+        <v>if ($('#dparameters').html().trim()==19) { var dataparameter=[['OAT','left','Common zone','Outdoor-Air Temp (temp)'],['OADPS','right','Air handle unit','Outdoor-Air Damper Position Signal (%)'],['OAF','right','Air handle unit','Outdoor-Air Fraction temp'],['OM','right','Common zone','Occupancy Mode']]; }</v>
       </c>
       <c r="H29" t="s">
         <v>11</v>
@@ -4001,19 +4332,19 @@
       </c>
       <c r="R29" s="4" t="str">
         <f>IF(H29&lt;&gt;"",VLOOKUP(H29,Tabla1[#All],3,FALSE),"")</f>
-        <v>Outdoor-Air Temp (temp)</v>
+        <v>Common zone</v>
       </c>
       <c r="S29" s="4" t="str">
         <f>IF(I29&lt;&gt;"",VLOOKUP(I29,Tabla1[#All],3,FALSE),"")</f>
-        <v>Outdoor-Air Damper Position Signal (%)</v>
+        <v>Air handle unit</v>
       </c>
       <c r="T29" s="4" t="str">
         <f>IF(J29&lt;&gt;"",VLOOKUP(J29,Tabla1[#All],3,FALSE),"")</f>
-        <v>Outdoor-Air Fraction temp</v>
+        <v>Air handle unit</v>
       </c>
       <c r="U29" s="4" t="str">
         <f>IF(K29&lt;&gt;"",VLOOKUP(K29,Tabla1[#All],3,FALSE),"")</f>
-        <v>Occupancy Mode</v>
+        <v>Common zone</v>
       </c>
       <c r="V29" s="4" t="str">
         <f>IF(L29&lt;&gt;"",VLOOKUP(L29,Tabla1[#All],3,FALSE),"")</f>
@@ -4021,19 +4352,19 @@
       </c>
       <c r="W29" s="1" t="str">
         <f>IF(H29&lt;&gt;"",VLOOKUP(H29,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Outdoor-Air Temp (temp)</v>
       </c>
       <c r="X29" s="1" t="str">
         <f>IF(I29&lt;&gt;"",VLOOKUP(I29,Tabla1[#All],4,FALSE),"")</f>
-        <v>column</v>
+        <v>Outdoor-Air Damper Position Signal (%)</v>
       </c>
       <c r="Y29" s="1" t="str">
         <f>IF(J29&lt;&gt;"",VLOOKUP(J29,Tabla1[#All],4,FALSE),"")</f>
-        <v>column</v>
+        <v>Outdoor-Air Fraction temp</v>
       </c>
       <c r="Z29" s="1" t="str">
         <f>IF(K29&lt;&gt;"",VLOOKUP(K29,Tabla1[#All],4,FALSE),"")</f>
-        <v>column</v>
+        <v>Occupancy Mode</v>
       </c>
       <c r="AA29" s="1" t="str">
         <f>IF(L29&lt;&gt;"",VLOOKUP(L29,Tabla1[#All],4,FALSE),"")</f>
@@ -4041,19 +4372,19 @@
       </c>
       <c r="AB29" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>['OAT','left','Outdoor-Air Temp (temp)','smoothedLine']</v>
+        <v>['OAT','left','Common zone','Outdoor-Air Temp (temp)']</v>
       </c>
       <c r="AC29" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>,['OADPS','right','Outdoor-Air Damper Position Signal (%)','column']</v>
+        <v>,['OADPS','right','Air handle unit','Outdoor-Air Damper Position Signal (%)']</v>
       </c>
       <c r="AD29" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>,['OAF','right','Outdoor-Air Fraction temp','column']</v>
+        <v>,['OAF','right','Air handle unit','Outdoor-Air Fraction temp']</v>
       </c>
       <c r="AE29" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>,['OM','right','Occupancy Mode','column']</v>
+        <v>,['OM','right','Common zone','Occupancy Mode']</v>
       </c>
       <c r="AF29" s="3" t="str">
         <f t="shared" si="2"/>
@@ -4066,7 +4397,7 @@
       </c>
       <c r="B30" t="str">
         <f t="shared" si="0"/>
-        <v>if ($('#dparameters').html().trim()==20) { var dataparameter=[['OAT','left','Outdoor-Air Temp (temp)','smoothedLine'],['OADPS','right','Outdoor-Air Damper Position Signal (%)','column'],['OM','right','Occupancy Mode','column']]; }</v>
+        <v>if ($('#dparameters').html().trim()==20) { var dataparameter=[['OAT','left','Common zone','Outdoor-Air Temp (temp)'],['OADPS','right','Air handle unit','Outdoor-Air Damper Position Signal (%)'],['OM','right','Common zone','Occupancy Mode']]; }</v>
       </c>
       <c r="H30" t="s">
         <v>11</v>
@@ -4099,15 +4430,15 @@
       </c>
       <c r="R30" s="4" t="str">
         <f>IF(H30&lt;&gt;"",VLOOKUP(H30,Tabla1[#All],3,FALSE),"")</f>
-        <v>Outdoor-Air Temp (temp)</v>
+        <v>Common zone</v>
       </c>
       <c r="S30" s="4" t="str">
         <f>IF(I30&lt;&gt;"",VLOOKUP(I30,Tabla1[#All],3,FALSE),"")</f>
-        <v>Outdoor-Air Damper Position Signal (%)</v>
+        <v>Air handle unit</v>
       </c>
       <c r="T30" s="4" t="str">
         <f>IF(J30&lt;&gt;"",VLOOKUP(J30,Tabla1[#All],3,FALSE),"")</f>
-        <v>Occupancy Mode</v>
+        <v>Common zone</v>
       </c>
       <c r="U30" s="4" t="str">
         <f>IF(K30&lt;&gt;"",VLOOKUP(K30,Tabla1[#All],3,FALSE),"")</f>
@@ -4119,15 +4450,15 @@
       </c>
       <c r="W30" s="1" t="str">
         <f>IF(H30&lt;&gt;"",VLOOKUP(H30,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Outdoor-Air Temp (temp)</v>
       </c>
       <c r="X30" s="1" t="str">
         <f>IF(I30&lt;&gt;"",VLOOKUP(I30,Tabla1[#All],4,FALSE),"")</f>
-        <v>column</v>
+        <v>Outdoor-Air Damper Position Signal (%)</v>
       </c>
       <c r="Y30" s="1" t="str">
         <f>IF(J30&lt;&gt;"",VLOOKUP(J30,Tabla1[#All],4,FALSE),"")</f>
-        <v>column</v>
+        <v>Occupancy Mode</v>
       </c>
       <c r="Z30" s="1" t="str">
         <f>IF(K30&lt;&gt;"",VLOOKUP(K30,Tabla1[#All],4,FALSE),"")</f>
@@ -4139,15 +4470,15 @@
       </c>
       <c r="AB30" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>['OAT','left','Outdoor-Air Temp (temp)','smoothedLine']</v>
+        <v>['OAT','left','Common zone','Outdoor-Air Temp (temp)']</v>
       </c>
       <c r="AC30" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>,['OADPS','right','Outdoor-Air Damper Position Signal (%)','column']</v>
+        <v>,['OADPS','right','Air handle unit','Outdoor-Air Damper Position Signal (%)']</v>
       </c>
       <c r="AD30" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>,['OM','right','Occupancy Mode','column']</v>
+        <v>,['OM','right','Common zone','Occupancy Mode']</v>
       </c>
       <c r="AE30" s="3" t="str">
         <f t="shared" si="2"/>
@@ -4164,7 +4495,7 @@
       </c>
       <c r="B31" t="str">
         <f t="shared" si="0"/>
-        <v>if ($('#dparameters').html().trim()==21) { var dataparameter=[['DSP','left','Duct Static Pressure','smoothedLine'],['DSPSP','left','Duct Static Pressure Set Point','smoothedLine']]; }</v>
+        <v>if ($('#dparameters').html().trim()==21) { var dataparameter=[['DSP','left','Air handle unit','Duct Static Pressure'],['DSPSP','left','Air handle unit','Duct Static Pressure Set Point']]; }</v>
       </c>
       <c r="H31" t="s">
         <v>6</v>
@@ -4194,11 +4525,11 @@
       </c>
       <c r="R31" s="4" t="str">
         <f>IF(H31&lt;&gt;"",VLOOKUP(H31,Tabla1[#All],3,FALSE),"")</f>
-        <v>Duct Static Pressure</v>
+        <v>Air handle unit</v>
       </c>
       <c r="S31" s="4" t="str">
         <f>IF(I31&lt;&gt;"",VLOOKUP(I31,Tabla1[#All],3,FALSE),"")</f>
-        <v>Duct Static Pressure Set Point</v>
+        <v>Air handle unit</v>
       </c>
       <c r="T31" s="4" t="str">
         <f>IF(J31&lt;&gt;"",VLOOKUP(J31,Tabla1[#All],3,FALSE),"")</f>
@@ -4214,11 +4545,11 @@
       </c>
       <c r="W31" s="1" t="str">
         <f>IF(H31&lt;&gt;"",VLOOKUP(H31,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Duct Static Pressure</v>
       </c>
       <c r="X31" s="1" t="str">
         <f>IF(I31&lt;&gt;"",VLOOKUP(I31,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Duct Static Pressure Set Point</v>
       </c>
       <c r="Y31" s="1" t="str">
         <f>IF(J31&lt;&gt;"",VLOOKUP(J31,Tabla1[#All],4,FALSE),"")</f>
@@ -4234,11 +4565,11 @@
       </c>
       <c r="AB31" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>['DSP','left','Duct Static Pressure','smoothedLine']</v>
+        <v>['DSP','left','Air handle unit','Duct Static Pressure']</v>
       </c>
       <c r="AC31" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>,['DSPSP','left','Duct Static Pressure Set Point','smoothedLine']</v>
+        <v>,['DSPSP','left','Air handle unit','Duct Static Pressure Set Point']</v>
       </c>
       <c r="AD31" s="3" t="str">
         <f t="shared" si="2"/>
@@ -4259,7 +4590,7 @@
       </c>
       <c r="B32" t="str">
         <f t="shared" si="0"/>
-        <v>if ($('#dparameters').html().trim()==22) { var dataparameter=[['DSP','left','Duct Static Pressure','smoothedLine']]; }</v>
+        <v>if ($('#dparameters').html().trim()==22) { var dataparameter=[['DSP','left','Air handle unit','Duct Static Pressure']]; }</v>
       </c>
       <c r="H32" t="s">
         <v>6</v>
@@ -4286,7 +4617,7 @@
       </c>
       <c r="R32" s="4" t="str">
         <f>IF(H32&lt;&gt;"",VLOOKUP(H32,Tabla1[#All],3,FALSE),"")</f>
-        <v>Duct Static Pressure</v>
+        <v>Air handle unit</v>
       </c>
       <c r="S32" s="4" t="str">
         <f>IF(I32&lt;&gt;"",VLOOKUP(I32,Tabla1[#All],3,FALSE),"")</f>
@@ -4306,7 +4637,7 @@
       </c>
       <c r="W32" s="1" t="str">
         <f>IF(H32&lt;&gt;"",VLOOKUP(H32,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Duct Static Pressure</v>
       </c>
       <c r="X32" s="1" t="str">
         <f>IF(I32&lt;&gt;"",VLOOKUP(I32,Tabla1[#All],4,FALSE),"")</f>
@@ -4326,7 +4657,7 @@
       </c>
       <c r="AB32" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>['DSP','left','Duct Static Pressure','smoothedLine']</v>
+        <v>['DSP','left','Air handle unit','Duct Static Pressure']</v>
       </c>
       <c r="AC32" s="3" t="str">
         <f t="shared" si="2"/>
@@ -4351,7 +4682,7 @@
       </c>
       <c r="B33" t="str">
         <f t="shared" si="0"/>
-        <v>if ($('#dparameters').html().trim()==23) { var dataparameter=[['VAVDPSP','right','VAV Damper Position Set Point (%)','column']]; }</v>
+        <v>if ($('#dparameters').html().trim()==23) { var dataparameter=[['VAVDPSP','right','0','VAV Damper Position Set Point (%)']]; }</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>34</v>
@@ -4376,9 +4707,9 @@
         <f>IF(L33&lt;&gt;"",VLOOKUP(L33,Tabla1[#All],2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="R33" s="4" t="str">
+      <c r="R33" s="4">
         <f>IF(H33&lt;&gt;"",VLOOKUP(H33,Tabla1[#All],3,FALSE),"")</f>
-        <v>VAV Damper Position Set Point (%)</v>
+        <v>0</v>
       </c>
       <c r="S33" s="4" t="str">
         <f>IF(I33&lt;&gt;"",VLOOKUP(I33,Tabla1[#All],3,FALSE),"")</f>
@@ -4398,7 +4729,7 @@
       </c>
       <c r="W33" s="1" t="str">
         <f>IF(H33&lt;&gt;"",VLOOKUP(H33,Tabla1[#All],4,FALSE),"")</f>
-        <v>column</v>
+        <v>VAV Damper Position Set Point (%)</v>
       </c>
       <c r="X33" s="1" t="str">
         <f>IF(I33&lt;&gt;"",VLOOKUP(I33,Tabla1[#All],4,FALSE),"")</f>
@@ -4418,7 +4749,7 @@
       </c>
       <c r="AB33" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>['VAVDPSP','right','VAV Damper Position Set Point (%)','column']</v>
+        <v>['VAVDPSP','right','0','VAV Damper Position Set Point (%)']</v>
       </c>
       <c r="AC33" s="3" t="str">
         <f t="shared" si="2"/>
@@ -4443,7 +4774,7 @@
       </c>
       <c r="B34" t="str">
         <f t="shared" si="0"/>
-        <v>if ($('#dparameters').html().trim()==24) { var dataparameter=[['DAT','left','Discharge-Air Temp','smoothedLine'],['DATSP','left','Discharge-Air Temp Set Point','smoothedLine']]; }</v>
+        <v>if ($('#dparameters').html().trim()==24) { var dataparameter=[['DAT','left','Air handle unit','Discharge-Air Temp'],['DATSP','left','Air handle unit','Discharge-Air Temp Set Point']]; }</v>
       </c>
       <c r="H34" t="s">
         <v>13</v>
@@ -4473,11 +4804,11 @@
       </c>
       <c r="R34" s="4" t="str">
         <f>IF(H34&lt;&gt;"",VLOOKUP(H34,Tabla1[#All],3,FALSE),"")</f>
-        <v>Discharge-Air Temp</v>
+        <v>Air handle unit</v>
       </c>
       <c r="S34" s="4" t="str">
         <f>IF(I34&lt;&gt;"",VLOOKUP(I34,Tabla1[#All],3,FALSE),"")</f>
-        <v>Discharge-Air Temp Set Point</v>
+        <v>Air handle unit</v>
       </c>
       <c r="T34" s="4" t="str">
         <f>IF(J34&lt;&gt;"",VLOOKUP(J34,Tabla1[#All],3,FALSE),"")</f>
@@ -4493,11 +4824,11 @@
       </c>
       <c r="W34" s="1" t="str">
         <f>IF(H34&lt;&gt;"",VLOOKUP(H34,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Discharge-Air Temp</v>
       </c>
       <c r="X34" s="1" t="str">
         <f>IF(I34&lt;&gt;"",VLOOKUP(I34,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Discharge-Air Temp Set Point</v>
       </c>
       <c r="Y34" s="1" t="str">
         <f>IF(J34&lt;&gt;"",VLOOKUP(J34,Tabla1[#All],4,FALSE),"")</f>
@@ -4513,11 +4844,11 @@
       </c>
       <c r="AB34" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>['DAT','left','Discharge-Air Temp','smoothedLine']</v>
+        <v>['DAT','left','Air handle unit','Discharge-Air Temp']</v>
       </c>
       <c r="AC34" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>,['DATSP','left','Discharge-Air Temp Set Point','smoothedLine']</v>
+        <v>,['DATSP','left','Air handle unit','Discharge-Air Temp Set Point']</v>
       </c>
       <c r="AD34" s="3" t="str">
         <f t="shared" si="2"/>
@@ -4538,7 +4869,7 @@
       </c>
       <c r="B35" t="str">
         <f t="shared" si="0"/>
-        <v>if ($('#dparameters').html().trim()==25) { var dataparameter=[['DAT','left','Discharge-Air Temp','smoothedLine'],['DATSP','left','Discharge-Air Temp Set Point','smoothedLine'],['OAT','left','Outdoor-Air Temp (temp)','smoothedLine']]; }</v>
+        <v>if ($('#dparameters').html().trim()==25) { var dataparameter=[['DAT','left','Air handle unit','Discharge-Air Temp'],['DATSP','left','Air handle unit','Discharge-Air Temp Set Point'],['OAT','left','Common zone','Outdoor-Air Temp (temp)']]; }</v>
       </c>
       <c r="H35" t="s">
         <v>13</v>
@@ -4571,15 +4902,15 @@
       </c>
       <c r="R35" s="4" t="str">
         <f>IF(H35&lt;&gt;"",VLOOKUP(H35,Tabla1[#All],3,FALSE),"")</f>
-        <v>Discharge-Air Temp</v>
+        <v>Air handle unit</v>
       </c>
       <c r="S35" s="4" t="str">
         <f>IF(I35&lt;&gt;"",VLOOKUP(I35,Tabla1[#All],3,FALSE),"")</f>
-        <v>Discharge-Air Temp Set Point</v>
+        <v>Air handle unit</v>
       </c>
       <c r="T35" s="4" t="str">
         <f>IF(J35&lt;&gt;"",VLOOKUP(J35,Tabla1[#All],3,FALSE),"")</f>
-        <v>Outdoor-Air Temp (temp)</v>
+        <v>Common zone</v>
       </c>
       <c r="U35" s="4" t="str">
         <f>IF(K35&lt;&gt;"",VLOOKUP(K35,Tabla1[#All],3,FALSE),"")</f>
@@ -4591,15 +4922,15 @@
       </c>
       <c r="W35" s="1" t="str">
         <f>IF(H35&lt;&gt;"",VLOOKUP(H35,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Discharge-Air Temp</v>
       </c>
       <c r="X35" s="1" t="str">
         <f>IF(I35&lt;&gt;"",VLOOKUP(I35,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Discharge-Air Temp Set Point</v>
       </c>
       <c r="Y35" s="1" t="str">
         <f>IF(J35&lt;&gt;"",VLOOKUP(J35,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Outdoor-Air Temp (temp)</v>
       </c>
       <c r="Z35" s="1" t="str">
         <f>IF(K35&lt;&gt;"",VLOOKUP(K35,Tabla1[#All],4,FALSE),"")</f>
@@ -4611,15 +4942,15 @@
       </c>
       <c r="AB35" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>['DAT','left','Discharge-Air Temp','smoothedLine']</v>
+        <v>['DAT','left','Air handle unit','Discharge-Air Temp']</v>
       </c>
       <c r="AC35" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>,['DATSP','left','Discharge-Air Temp Set Point','smoothedLine']</v>
+        <v>,['DATSP','left','Air handle unit','Discharge-Air Temp Set Point']</v>
       </c>
       <c r="AD35" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>,['OAT','left','Outdoor-Air Temp (temp)','smoothedLine']</v>
+        <v>,['OAT','left','Common zone','Outdoor-Air Temp (temp)']</v>
       </c>
       <c r="AE35" s="3" t="str">
         <f t="shared" si="2"/>
@@ -4636,7 +4967,7 @@
       </c>
       <c r="B36" t="str">
         <f t="shared" si="0"/>
-        <v>if ($('#dparameters').html().trim()==26) { var dataparameter=[['ZRVS','right','Zone Reheat Valve Signal (%)','column']]; }</v>
+        <v>if ($('#dparameters').html().trim()==26) { var dataparameter=[['ZRVS','right','Common zone','Zone Reheat Valve Signal (%)']]; }</v>
       </c>
       <c r="H36" t="s">
         <v>7</v>
@@ -4663,7 +4994,7 @@
       </c>
       <c r="R36" s="4" t="str">
         <f>IF(H36&lt;&gt;"",VLOOKUP(H36,Tabla1[#All],3,FALSE),"")</f>
-        <v>Zone Reheat Valve Signal (%)</v>
+        <v>Common zone</v>
       </c>
       <c r="S36" s="4" t="str">
         <f>IF(I36&lt;&gt;"",VLOOKUP(I36,Tabla1[#All],3,FALSE),"")</f>
@@ -4683,7 +5014,7 @@
       </c>
       <c r="W36" s="1" t="str">
         <f>IF(H36&lt;&gt;"",VLOOKUP(H36,Tabla1[#All],4,FALSE),"")</f>
-        <v>column</v>
+        <v>Zone Reheat Valve Signal (%)</v>
       </c>
       <c r="X36" s="1" t="str">
         <f>IF(I36&lt;&gt;"",VLOOKUP(I36,Tabla1[#All],4,FALSE),"")</f>
@@ -4703,7 +5034,7 @@
       </c>
       <c r="AB36" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>['ZRVS','right','Zone Reheat Valve Signal (%)','column']</v>
+        <v>['ZRVS','right','Common zone','Zone Reheat Valve Signal (%)']</v>
       </c>
       <c r="AC36" s="3" t="str">
         <f t="shared" si="2"/>
@@ -4728,7 +5059,7 @@
       </c>
       <c r="B37" t="str">
         <f t="shared" si="0"/>
-        <v>if ($('#dparameters').html().trim()==27) { var dataparameter=[['DSP','left','Duct Static Pressure','smoothedLine']]; }</v>
+        <v>if ($('#dparameters').html().trim()==27) { var dataparameter=[['DSP','left','Air handle unit','Duct Static Pressure']]; }</v>
       </c>
       <c r="H37" t="s">
         <v>6</v>
@@ -4755,7 +5086,7 @@
       </c>
       <c r="R37" s="4" t="str">
         <f>IF(H37&lt;&gt;"",VLOOKUP(H37,Tabla1[#All],3,FALSE),"")</f>
-        <v>Duct Static Pressure</v>
+        <v>Air handle unit</v>
       </c>
       <c r="S37" s="4" t="str">
         <f>IF(I37&lt;&gt;"",VLOOKUP(I37,Tabla1[#All],3,FALSE),"")</f>
@@ -4775,7 +5106,7 @@
       </c>
       <c r="W37" s="1" t="str">
         <f>IF(H37&lt;&gt;"",VLOOKUP(H37,Tabla1[#All],4,FALSE),"")</f>
-        <v>smoothedLine</v>
+        <v>Duct Static Pressure</v>
       </c>
       <c r="X37" s="1" t="str">
         <f>IF(I37&lt;&gt;"",VLOOKUP(I37,Tabla1[#All],4,FALSE),"")</f>
@@ -4795,7 +5126,7 @@
       </c>
       <c r="AB37" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>['DSP','left','Duct Static Pressure','smoothedLine']</v>
+        <v>['DSP','left','Air handle unit','Duct Static Pressure']</v>
       </c>
       <c r="AC37" s="3" t="str">
         <f t="shared" si="2"/>
@@ -4820,7 +5151,7 @@
       </c>
       <c r="B38" t="str">
         <f t="shared" si="0"/>
-        <v>if ($('#dparameters').html().trim()==28) { var dataparameter=[['SFS','right','Supply Fan Status (on/off)','column']]; }</v>
+        <v>if ($('#dparameters').html().trim()==28) { var dataparameter=[['SFS','right','Air handle unit','Supply Fan Status (on/off)']]; }</v>
       </c>
       <c r="H38" t="s">
         <v>8</v>
@@ -4847,7 +5178,7 @@
       </c>
       <c r="R38" s="4" t="str">
         <f>IF(H38&lt;&gt;"",VLOOKUP(H38,Tabla1[#All],3,FALSE),"")</f>
-        <v>Supply Fan Status (on/off)</v>
+        <v>Air handle unit</v>
       </c>
       <c r="S38" s="4" t="str">
         <f>IF(I38&lt;&gt;"",VLOOKUP(I38,Tabla1[#All],3,FALSE),"")</f>
@@ -4867,7 +5198,7 @@
       </c>
       <c r="W38" s="1" t="str">
         <f>IF(H38&lt;&gt;"",VLOOKUP(H38,Tabla1[#All],4,FALSE),"")</f>
-        <v>column</v>
+        <v>Supply Fan Status (on/off)</v>
       </c>
       <c r="X38" s="1" t="str">
         <f>IF(I38&lt;&gt;"",VLOOKUP(I38,Tabla1[#All],4,FALSE),"")</f>
@@ -4887,7 +5218,7 @@
       </c>
       <c r="AB38" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>['SFS','right','Supply Fan Status (on/off)','column']</v>
+        <v>['SFS','right','Air handle unit','Supply Fan Status (on/off)']</v>
       </c>
       <c r="AC38" s="3" t="str">
         <f t="shared" si="2"/>

</xml_diff>